<commit_message>
update for 27 feb
</commit_message>
<xml_diff>
--- a/Manual/input-data.xlsx
+++ b/Manual/input-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibhav/Documents/Projects/nimf-tracker-git/nimf-tracker/Manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5259786E-2212-424C-94C2-D3F5BB385437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109C2AA3-8173-6C47-9D86-CEF5A7AAD63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="6840" windowWidth="17060" windowHeight="9960" firstSheet="4" activeTab="6" xr2:uid="{D619B3DC-10A9-6C4B-8E47-54B1B3814066}"/>
+    <workbookView xWindow="34140" yWindow="10460" windowWidth="17060" windowHeight="9960" firstSheet="13" activeTab="19" xr2:uid="{D619B3DC-10A9-6C4B-8E47-54B1B3814066}"/>
   </bookViews>
   <sheets>
     <sheet name="gst-eway" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="210">
   <si>
     <t>e-Way</t>
   </si>
@@ -443,199 +443,19 @@
     <t>7 </t>
   </si>
   <si>
-    <t>11 </t>
-  </si>
-  <si>
     <t>9 </t>
-  </si>
-  <si>
-    <t>1088 </t>
   </si>
   <si>
     <t>Kerala***</t>
   </si>
   <si>
-    <t>87 </t>
-  </si>
-  <si>
-    <t>23 </t>
-  </si>
-  <si>
-    <t>158 </t>
-  </si>
-  <si>
-    <t>20 </t>
-  </si>
-  <si>
-    <t>21 </t>
-  </si>
-  <si>
-    <t>22 </t>
-  </si>
-  <si>
-    <t>1063 </t>
-  </si>
-  <si>
-    <t>1486 </t>
-  </si>
-  <si>
-    <t>29 </t>
-  </si>
-  <si>
-    <t>55 </t>
-  </si>
-  <si>
-    <t>153 </t>
-  </si>
-  <si>
-    <t>179 </t>
-  </si>
-  <si>
     <t>80 </t>
-  </si>
-  <si>
-    <t>151 </t>
-  </si>
-  <si>
-    <t>62 </t>
-  </si>
-  <si>
-    <t>317 </t>
-  </si>
-  <si>
-    <t>821 </t>
-  </si>
-  <si>
-    <t>791 </t>
-  </si>
-  <si>
-    <t>130 </t>
-  </si>
-  <si>
-    <t>199 </t>
-  </si>
-  <si>
-    <t>946 </t>
-  </si>
-  <si>
-    <t>1419 </t>
-  </si>
-  <si>
-    <t>313 </t>
-  </si>
-  <si>
-    <t>867 </t>
-  </si>
-  <si>
-    <t>305 </t>
   </si>
   <si>
     <t>303 </t>
   </si>
   <si>
-    <t>469 </t>
-  </si>
-  <si>
-    <t>91 </t>
-  </si>
-  <si>
-    <t>173 </t>
-  </si>
-  <si>
-    <t>2753 </t>
-  </si>
-  <si>
-    <t>3870 </t>
-  </si>
-  <si>
-    <t>10853 </t>
-  </si>
-  <si>
-    <t>17086 </t>
-  </si>
-  <si>
-    <t>112 </t>
-  </si>
-  <si>
-    <t>1342 </t>
-  </si>
-  <si>
-    <t>2353 </t>
-  </si>
-  <si>
-    <t>2788 </t>
-  </si>
-  <si>
-    <t>4394 </t>
-  </si>
-  <si>
-    <t>76 </t>
-  </si>
-  <si>
-    <t>105 </t>
-  </si>
-  <si>
-    <t>152 </t>
-  </si>
-  <si>
-    <t>1173 </t>
-  </si>
-  <si>
-    <t>36 </t>
-  </si>
-  <si>
-    <t>750 </t>
-  </si>
-  <si>
-    <t>1266 </t>
-  </si>
-  <si>
     <t>18 </t>
-  </si>
-  <si>
-    <t>121 </t>
-  </si>
-  <si>
-    <t>269 </t>
-  </si>
-  <si>
-    <t>449 </t>
-  </si>
-  <si>
-    <t>1233 </t>
-  </si>
-  <si>
-    <t>2299 </t>
-  </si>
-  <si>
-    <t>2517 </t>
-  </si>
-  <si>
-    <t>3561 </t>
-  </si>
-  <si>
-    <t>465 </t>
-  </si>
-  <si>
-    <t>865 </t>
-  </si>
-  <si>
-    <t>17 </t>
-  </si>
-  <si>
-    <t>541 </t>
-  </si>
-  <si>
-    <t>783 </t>
-  </si>
-  <si>
-    <t>1131 </t>
-  </si>
-  <si>
-    <t>1902 </t>
-  </si>
-  <si>
-    <t>1357 </t>
   </si>
   <si>
     <t>Domestic</t>
@@ -700,6 +520,168 @@
   <si>
     <t>Grand Total</t>
   </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>218 </t>
+  </si>
+  <si>
+    <t>496 </t>
+  </si>
+  <si>
+    <t>43 </t>
+  </si>
+  <si>
+    <t>59 </t>
+  </si>
+  <si>
+    <t>56 </t>
+  </si>
+  <si>
+    <t>73 </t>
+  </si>
+  <si>
+    <t>31 </t>
+  </si>
+  <si>
+    <t>100 </t>
+  </si>
+  <si>
+    <t>315 </t>
+  </si>
+  <si>
+    <t>191 </t>
+  </si>
+  <si>
+    <t>649 </t>
+  </si>
+  <si>
+    <t>60 </t>
+  </si>
+  <si>
+    <t>90 </t>
+  </si>
+  <si>
+    <t>404 </t>
+  </si>
+  <si>
+    <t>644 </t>
+  </si>
+  <si>
+    <t>190 </t>
+  </si>
+  <si>
+    <t>585 </t>
+  </si>
+  <si>
+    <t>149 </t>
+  </si>
+  <si>
+    <t>297 </t>
+  </si>
+  <si>
+    <t>92 </t>
+  </si>
+  <si>
+    <t>187 </t>
+  </si>
+  <si>
+    <t>33 </t>
+  </si>
+  <si>
+    <t>85 </t>
+  </si>
+  <si>
+    <t>736 </t>
+  </si>
+  <si>
+    <t>1349 </t>
+  </si>
+  <si>
+    <t>15 </t>
+  </si>
+  <si>
+    <t>4433 </t>
+  </si>
+  <si>
+    <t>7837 </t>
+  </si>
+  <si>
+    <t>49 </t>
+  </si>
+  <si>
+    <t>42 </t>
+  </si>
+  <si>
+    <t>361 </t>
+  </si>
+  <si>
+    <t>889 </t>
+  </si>
+  <si>
+    <t>1560 </t>
+  </si>
+  <si>
+    <t>2521 </t>
+  </si>
+  <si>
+    <t>27 </t>
+  </si>
+  <si>
+    <t>10 </t>
+  </si>
+  <si>
+    <t>34 </t>
+  </si>
+  <si>
+    <t>1207 </t>
+  </si>
+  <si>
+    <t>247 </t>
+  </si>
+  <si>
+    <t>39 </t>
+  </si>
+  <si>
+    <t>51 </t>
+  </si>
+  <si>
+    <t>164 </t>
+  </si>
+  <si>
+    <t>857 </t>
+  </si>
+  <si>
+    <t>1510 </t>
+  </si>
+  <si>
+    <t>1290 </t>
+  </si>
+  <si>
+    <t>1794 </t>
+  </si>
+  <si>
+    <t>282 </t>
+  </si>
+  <si>
+    <t>569 </t>
+  </si>
+  <si>
+    <t>106 </t>
+  </si>
+  <si>
+    <t>357 </t>
+  </si>
+  <si>
+    <t>823 </t>
+  </si>
+  <si>
+    <t>174 </t>
+  </si>
+  <si>
+    <t>430 </t>
+  </si>
 </sst>
 </file>
 
@@ -709,7 +691,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -808,18 +790,40 @@
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Source Sans Pro"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Source Sans Pro"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF333333"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -863,9 +867,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -897,7 +901,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -907,6 +910,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1519,7 +1529,7 @@
         <v>44593</v>
       </c>
       <c r="B27">
-        <v>30670233</v>
+        <v>47656893</v>
       </c>
       <c r="C27" s="17"/>
     </row>
@@ -1532,7 +1542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8730D1-B073-F949-92E6-FAE69CFEA773}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A63" workbookViewId="0">
       <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
@@ -5000,7 +5010,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
+      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6232,11 +6242,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F84EB-1F73-1245-BB50-FDD52D41BDBE}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
+      <selection pane="bottomLeft" activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6943,6 +6953,17 @@
       </c>
       <c r="C64">
         <v>8.27</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="3">
+        <v>44603</v>
+      </c>
+      <c r="B65" s="5">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="C65" s="5">
+        <v>8.3800000000000008</v>
       </c>
     </row>
   </sheetData>
@@ -6955,7 +6976,7 @@
   <dimension ref="A1:B130"/>
   <sheetViews>
     <sheetView topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126"/>
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7996,7 +8017,12 @@
       </c>
     </row>
     <row r="130" spans="1:2">
-      <c r="B130" s="17"/>
+      <c r="A130" s="3">
+        <v>44610</v>
+      </c>
+      <c r="B130" s="17">
+        <v>45508670</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8005,7 +8031,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5353B576-38C4-E445-9E6D-988228532D05}">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
@@ -9059,6 +9085,17 @@
         <v>8.2100000000000009</v>
       </c>
     </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="26">
+        <v>44603</v>
+      </c>
+      <c r="B96" s="5">
+        <v>9.11</v>
+      </c>
+      <c r="C96" s="5">
+        <v>7.86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9066,15 +9103,13 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F0D774-4FB9-484A-8B9C-C85D078E33FB}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -9088,21 +9123,21 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="18">
+    <row r="2" spans="1:15" ht="18">
       <c r="A2" s="20" t="s">
         <v>68</v>
       </c>
       <c r="B2" s="20">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
       <c r="D2" s="20">
-        <v>9833</v>
+        <v>9872</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="F2" s="20">
         <v>129</v>
@@ -9110,32 +9145,31 @@
       <c r="G2" s="20"/>
       <c r="H2" s="22"/>
       <c r="I2" s="22"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="20"/>
       <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
+      <c r="N2" s="22"/>
       <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-    </row>
-    <row r="3" spans="1:16" ht="18">
+    </row>
+    <row r="3" spans="1:15" ht="18">
       <c r="A3" s="20" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="20">
-        <v>7358</v>
+        <v>4709</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="D3" s="20">
-        <v>2293882</v>
+        <v>2298033</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="F3" s="20">
-        <v>14710</v>
+        <v>14722</v>
       </c>
       <c r="G3" s="22" t="s">
         <v>74</v>
@@ -9144,29 +9178,28 @@
       <c r="I3" s="22">
         <v>2</v>
       </c>
-      <c r="J3" s="21"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="22"/>
       <c r="N3" s="22"/>
       <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-    </row>
-    <row r="4" spans="1:16" ht="18">
+    </row>
+    <row r="4" spans="1:15" ht="18">
       <c r="A4" s="20" t="s">
         <v>71</v>
       </c>
       <c r="B4" s="20">
-        <v>322</v>
+        <v>178</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="D4" s="20">
-        <v>63652</v>
+        <v>63928</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="F4" s="20">
         <v>296</v>
@@ -9174,63 +9207,61 @@
       <c r="G4" s="20"/>
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="21"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="20"/>
       <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
+      <c r="N4" s="22"/>
       <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-    </row>
-    <row r="5" spans="1:16" ht="18">
+    </row>
+    <row r="5" spans="1:15" ht="18">
       <c r="A5" s="20" t="s">
         <v>72</v>
       </c>
       <c r="B5" s="20">
-        <v>2160</v>
+        <v>1610</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="D5" s="20">
-        <v>715147</v>
+        <v>715840</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="F5" s="20">
-        <v>6629</v>
+        <v>6638</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="22">
-        <v>3</v>
-      </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="20"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="22"/>
       <c r="N5" s="22"/>
       <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-    </row>
-    <row r="6" spans="1:16" ht="18">
+    </row>
+    <row r="6" spans="1:15" ht="18">
       <c r="A6" s="20" t="s">
         <v>73</v>
       </c>
       <c r="B6" s="20">
-        <v>703</v>
+        <v>349</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="D6" s="20">
-        <v>816661</v>
+        <v>817349</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="F6" s="20">
         <v>12255</v>
@@ -9238,89 +9269,90 @@
       <c r="G6" s="20"/>
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="22"/>
       <c r="N6" s="22"/>
       <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-    </row>
-    <row r="7" spans="1:16" ht="18">
+    </row>
+    <row r="7" spans="1:15" ht="18">
       <c r="A7" s="20" t="s">
         <v>62</v>
       </c>
       <c r="B7" s="20">
-        <v>249</v>
+        <v>167</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="D7" s="20">
-        <v>90136</v>
+        <v>90356</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="F7" s="20">
-        <v>1160</v>
+        <v>1164</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="22"/>
       <c r="N7" s="22"/>
       <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-    </row>
-    <row r="8" spans="1:16" ht="18">
+    </row>
+    <row r="8" spans="1:15" ht="18">
       <c r="A8" s="20" t="s">
         <v>75</v>
       </c>
       <c r="B8" s="20">
-        <v>3539</v>
+        <v>1961</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="D8" s="20">
-        <v>1131637</v>
+        <v>1134554</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="F8" s="20">
-        <v>14021</v>
-      </c>
-      <c r="G8" s="20"/>
+        <v>14024</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>78</v>
+      </c>
       <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="20"/>
+      <c r="I8" s="22">
+        <v>1</v>
+      </c>
+      <c r="J8" s="20"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="22"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-    </row>
-    <row r="9" spans="1:16" ht="18">
+    </row>
+    <row r="9" spans="1:15" ht="18">
       <c r="A9" s="20" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="20">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D9" s="20">
-        <v>11425</v>
+        <v>11433</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F9" s="20">
         <v>4</v>
@@ -9328,32 +9360,31 @@
       <c r="G9" s="20"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="21"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="20"/>
       <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
+      <c r="N9" s="22"/>
       <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-    </row>
-    <row r="10" spans="1:16" ht="18">
+    </row>
+    <row r="10" spans="1:15" ht="18">
       <c r="A10" s="20" t="s">
         <v>79</v>
       </c>
       <c r="B10" s="20">
-        <v>2617</v>
+        <v>2085</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>136</v>
+        <v>166</v>
       </c>
       <c r="D10" s="20">
-        <v>1826695</v>
+        <v>1830412</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="F10" s="20">
-        <v>26097</v>
+        <v>26117</v>
       </c>
       <c r="G10" s="22" t="s">
         <v>74</v>
@@ -9362,195 +9393,189 @@
       <c r="I10" s="22">
         <v>2</v>
       </c>
-      <c r="J10" s="21"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="22"/>
       <c r="N10" s="22"/>
       <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-    </row>
-    <row r="11" spans="1:16" ht="18">
+    </row>
+    <row r="11" spans="1:15" ht="18">
       <c r="A11" s="20" t="s">
         <v>80</v>
       </c>
       <c r="B11" s="20">
-        <v>677</v>
+        <v>347</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="D11" s="20">
-        <v>240207</v>
+        <v>240791</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="F11" s="20">
-        <v>3789</v>
+        <v>3800</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="22">
-        <v>1</v>
-      </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="22"/>
       <c r="N11" s="22"/>
       <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-    </row>
-    <row r="12" spans="1:16" ht="18">
+    </row>
+    <row r="12" spans="1:15" ht="18">
       <c r="A12" s="20" t="s">
         <v>81</v>
       </c>
       <c r="B12" s="20">
-        <v>5790</v>
+        <v>2538</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="D12" s="20">
-        <v>1203508</v>
+        <v>1208657</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="F12" s="20">
-        <v>10887</v>
+        <v>10924</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="22">
-        <v>13</v>
-      </c>
-      <c r="J12" s="21"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="21"/>
-      <c r="M12" s="20"/>
+        <v>5</v>
+      </c>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="22"/>
       <c r="N12" s="22"/>
       <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-    </row>
-    <row r="13" spans="1:16" ht="18">
+    </row>
+    <row r="13" spans="1:15" ht="18">
       <c r="A13" s="20" t="s">
         <v>82</v>
       </c>
       <c r="B13" s="20">
-        <v>3682</v>
+        <v>2310</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="D13" s="20">
-        <v>963666</v>
+        <v>967898</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="F13" s="20">
-        <v>10522</v>
+        <v>10551</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22">
-        <v>5</v>
-      </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="20"/>
+        <v>4</v>
+      </c>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="22"/>
       <c r="N13" s="22"/>
       <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-    </row>
-    <row r="14" spans="1:16" ht="18">
+    </row>
+    <row r="14" spans="1:15" ht="18">
       <c r="A14" s="20" t="s">
         <v>83</v>
       </c>
       <c r="B14" s="20">
-        <v>1992</v>
+        <v>1322</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="D14" s="20">
-        <v>275886</v>
+        <v>277637</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="F14" s="20">
-        <v>4093</v>
+        <v>4114</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="22">
-        <v>3</v>
-      </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="22"/>
       <c r="N14" s="22"/>
       <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
-    </row>
-    <row r="15" spans="1:16" ht="18">
+    </row>
+    <row r="15" spans="1:15" ht="18">
       <c r="A15" s="20" t="s">
         <v>84</v>
       </c>
       <c r="B15" s="20">
-        <v>2294</v>
+        <v>995</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="D15" s="20">
-        <v>445115</v>
+        <v>447074</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="F15" s="20">
-        <v>4746</v>
+        <v>4748</v>
       </c>
       <c r="G15" s="20"/>
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="22"/>
       <c r="N15" s="22"/>
       <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-    </row>
-    <row r="16" spans="1:16" ht="18">
+    </row>
+    <row r="16" spans="1:15" ht="18">
       <c r="A16" s="20" t="s">
         <v>85</v>
       </c>
       <c r="B16" s="20">
-        <v>746</v>
+        <v>520</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="D16" s="20">
-        <v>427869</v>
+        <v>428436</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F16" s="20">
         <v>5315</v>
@@ -9558,99 +9583,96 @@
       <c r="G16" s="20"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="21"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="20"/>
       <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
+      <c r="N16" s="22"/>
       <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
-    </row>
-    <row r="17" spans="1:16" ht="18">
+    </row>
+    <row r="17" spans="1:15" ht="18">
       <c r="A17" s="20" t="s">
         <v>86</v>
       </c>
       <c r="B17" s="20">
-        <v>13468</v>
+        <v>7556</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="D17" s="20">
-        <v>3882340</v>
+        <v>3892459</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="F17" s="20">
-        <v>39777</v>
+        <v>39900</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>137</v>
+        <v>182</v>
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="22">
-        <v>20</v>
-      </c>
-      <c r="J17" s="21"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="20"/>
+        <v>15</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="22"/>
       <c r="N17" s="22"/>
       <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-    </row>
-    <row r="18" spans="1:16" ht="18">
+    </row>
+    <row r="18" spans="1:15" ht="18">
       <c r="A18" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B18" s="20">
-        <v>75813</v>
+        <v>38040</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="D18" s="20">
-        <v>6323697</v>
+        <v>6388398</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="F18" s="20">
-        <v>64053</v>
+        <v>64980</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="H18" s="22">
-        <v>412</v>
+        <v>128</v>
       </c>
       <c r="I18" s="22">
-        <v>524</v>
-      </c>
-      <c r="J18" s="21"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="20"/>
+        <v>177</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="22"/>
       <c r="N18" s="22"/>
       <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-    </row>
-    <row r="19" spans="1:16" ht="18">
+    </row>
+    <row r="19" spans="1:15" ht="18">
       <c r="A19" s="20" t="s">
         <v>87</v>
       </c>
       <c r="B19" s="20">
-        <v>398</v>
+        <v>230</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="D19" s="20">
-        <v>27175</v>
+        <v>27513</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="F19" s="20">
         <v>228</v>
@@ -9658,29 +9680,28 @@
       <c r="G19" s="20"/>
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="21"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="20"/>
       <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
+      <c r="N19" s="22"/>
       <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-    </row>
-    <row r="20" spans="1:16" ht="18">
+    </row>
+    <row r="20" spans="1:15" ht="18">
       <c r="A20" s="20" t="s">
         <v>88</v>
       </c>
       <c r="B20" s="20">
-        <v>64</v>
+        <v>14</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="D20" s="20">
-        <v>11255</v>
+        <v>11331</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="F20" s="20">
         <v>52</v>
@@ -9688,32 +9709,31 @@
       <c r="G20" s="20"/>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="21"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="20"/>
       <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
+      <c r="N20" s="22"/>
       <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
-    </row>
-    <row r="21" spans="1:16" ht="18">
+    </row>
+    <row r="21" spans="1:15" ht="18">
       <c r="A21" s="20" t="s">
         <v>89</v>
       </c>
       <c r="B21" s="20">
-        <v>8364</v>
+        <v>4809</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="D21" s="20">
-        <v>1014413</v>
+        <v>1022161</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="F21" s="20">
-        <v>10713</v>
+        <v>10726</v>
       </c>
       <c r="G21" s="22" t="s">
         <v>74</v>
@@ -9722,100 +9742,97 @@
       <c r="I21" s="22">
         <v>2</v>
       </c>
-      <c r="J21" s="21"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="22"/>
       <c r="N21" s="22"/>
       <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
-    </row>
-    <row r="22" spans="1:16" ht="18">
+    </row>
+    <row r="22" spans="1:15" ht="18">
       <c r="A22" s="20" t="s">
         <v>91</v>
       </c>
       <c r="B22" s="20">
-        <v>22354</v>
+        <v>12682</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>170</v>
+        <v>189</v>
       </c>
       <c r="D22" s="20">
-        <v>7691064</v>
+        <v>7707254</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="F22" s="20">
-        <v>143576</v>
+        <v>143687</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="H22" s="22"/>
       <c r="I22" s="22">
-        <v>29</v>
-      </c>
-      <c r="J22" s="21"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="20"/>
+        <v>12</v>
+      </c>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="22"/>
       <c r="N22" s="22"/>
       <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
-    </row>
-    <row r="23" spans="1:16" ht="18">
+    </row>
+    <row r="23" spans="1:15" ht="18">
       <c r="A23" s="20" t="s">
         <v>92</v>
       </c>
       <c r="B23" s="20">
-        <v>683</v>
+        <v>536</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>90</v>
+        <v>191</v>
       </c>
       <c r="D23" s="20">
-        <v>133605</v>
+        <v>134046</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="F23" s="20">
-        <v>2096</v>
+        <v>2108</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="22">
-        <v>4</v>
-      </c>
-      <c r="J23" s="21"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="22"/>
       <c r="N23" s="22"/>
       <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-    </row>
-    <row r="24" spans="1:16" ht="18">
+    </row>
+    <row r="24" spans="1:15" ht="18">
       <c r="A24" s="20" t="s">
         <v>93</v>
       </c>
       <c r="B24" s="20">
-        <v>397</v>
+        <v>211</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="D24" s="20">
-        <v>91294</v>
+        <v>91627</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="F24" s="20">
-        <v>1568</v>
+        <v>1575</v>
       </c>
       <c r="G24" s="22" t="s">
         <v>74</v>
@@ -9824,327 +9841,305 @@
       <c r="I24" s="22">
         <v>2</v>
       </c>
-      <c r="J24" s="21"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="22"/>
       <c r="N24" s="22"/>
       <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-    </row>
-    <row r="25" spans="1:16" ht="18">
+    </row>
+    <row r="25" spans="1:15" ht="18">
       <c r="A25" s="20" t="s">
         <v>94</v>
       </c>
       <c r="B25" s="20">
-        <v>10071</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>174</v>
+        <v>8106</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>133</v>
       </c>
       <c r="D25" s="20">
-        <v>195089</v>
+        <v>203456</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="F25" s="20">
-        <v>642</v>
+        <v>655</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="H25" s="22"/>
       <c r="I25" s="22">
-        <v>1</v>
-      </c>
-      <c r="J25" s="21"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="J25" s="20"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="22"/>
       <c r="N25" s="22"/>
       <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-    </row>
-    <row r="26" spans="1:16" ht="18">
+    </row>
+    <row r="26" spans="1:15" ht="18">
       <c r="A26" s="20" t="s">
         <v>95</v>
       </c>
       <c r="B26" s="20">
-        <v>295</v>
+        <v>139</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="D26" s="20">
-        <v>34307</v>
+        <v>34502</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>176</v>
+        <v>134</v>
       </c>
       <c r="F26" s="20">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="22"/>
       <c r="N26" s="22"/>
       <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-    </row>
-    <row r="27" spans="1:16" ht="18">
+    </row>
+    <row r="27" spans="1:15" ht="18">
       <c r="A27" s="20" t="s">
         <v>96</v>
       </c>
       <c r="B27" s="20">
-        <v>5886</v>
+        <v>2843</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>177</v>
+        <v>195</v>
       </c>
       <c r="D27" s="20">
-        <v>1267109</v>
+        <v>1272428</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F27" s="20">
-        <v>8994</v>
+        <v>9052</v>
       </c>
       <c r="G27" s="22" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="H27" s="22"/>
       <c r="I27" s="22">
-        <v>18</v>
-      </c>
-      <c r="J27" s="21"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="J27" s="20"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="22"/>
       <c r="N27" s="22"/>
       <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-    </row>
-    <row r="28" spans="1:16" ht="18">
+    </row>
+    <row r="28" spans="1:15" ht="18">
       <c r="A28" s="20" t="s">
         <v>97</v>
       </c>
       <c r="B28" s="20">
-        <v>495</v>
+        <v>202</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>161</v>
+        <v>128</v>
       </c>
       <c r="D28" s="20">
-        <v>163110</v>
+        <v>163528</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F28" s="20">
-        <v>1959</v>
+        <v>1960</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="22"/>
       <c r="I28" s="22"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="22"/>
       <c r="N28" s="22"/>
       <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-    </row>
-    <row r="29" spans="1:16" ht="18">
+    </row>
+    <row r="29" spans="1:15" ht="18">
       <c r="A29" s="20" t="s">
         <v>98</v>
       </c>
       <c r="B29" s="20">
-        <v>1606</v>
+        <v>848</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="D29" s="20">
-        <v>737822</v>
+        <v>739310</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="F29" s="20">
-        <v>17662</v>
+        <v>17701</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="22">
-        <v>11</v>
-      </c>
-      <c r="J29" s="21"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="21"/>
-      <c r="M29" s="20"/>
+        <v>7</v>
+      </c>
+      <c r="J29" s="20"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="22"/>
       <c r="N29" s="22"/>
       <c r="O29" s="22"/>
-      <c r="P29" s="22"/>
-    </row>
-    <row r="30" spans="1:16" ht="18">
+    </row>
+    <row r="30" spans="1:15" ht="18">
       <c r="A30" s="20" t="s">
         <v>99</v>
       </c>
       <c r="B30" s="20">
-        <v>10967</v>
+        <v>5739</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="D30" s="20">
-        <v>1253305</v>
+        <v>1263081</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="F30" s="20">
-        <v>9516</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>131</v>
-      </c>
+        <v>9535</v>
+      </c>
+      <c r="G30" s="20"/>
       <c r="H30" s="22"/>
-      <c r="I30" s="22">
-        <v>9</v>
-      </c>
-      <c r="J30" s="21"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="20"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="22"/>
       <c r="N30" s="22"/>
       <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
-    </row>
-    <row r="31" spans="1:16" ht="18">
+    </row>
+    <row r="31" spans="1:15" ht="18">
       <c r="A31" s="20" t="s">
         <v>100</v>
       </c>
       <c r="B31" s="20">
-        <v>164</v>
+        <v>78</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="D31" s="20">
-        <v>38417</v>
+        <v>38540</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="F31" s="20">
-        <v>441</v>
-      </c>
-      <c r="G31" s="22" t="s">
-        <v>78</v>
-      </c>
+        <v>442</v>
+      </c>
+      <c r="G31" s="20"/>
       <c r="H31" s="22"/>
-      <c r="I31" s="22">
-        <v>1</v>
-      </c>
+      <c r="I31" s="22"/>
       <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="20"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="22"/>
       <c r="N31" s="22"/>
       <c r="O31" s="22"/>
-      <c r="P31" s="22"/>
-    </row>
-    <row r="32" spans="1:16" ht="18">
+    </row>
+    <row r="32" spans="1:15" ht="18">
       <c r="A32" s="20" t="s">
         <v>101</v>
       </c>
       <c r="B32" s="20">
-        <v>18164</v>
+        <v>8150</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="D32" s="20">
-        <v>3387839</v>
+        <v>3401938</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="F32" s="20">
-        <v>37977</v>
+        <v>38000</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="22">
-        <v>7</v>
-      </c>
-      <c r="J32" s="21"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="J32" s="20"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-    </row>
-    <row r="33" spans="1:16" ht="18">
+    </row>
+    <row r="33" spans="1:15" ht="18">
       <c r="A33" s="20" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="20">
-        <v>5646</v>
+        <v>3810</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="D33" s="20">
-        <v>776667</v>
+        <v>780462</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F33" s="20">
-        <v>4109</v>
-      </c>
-      <c r="G33" s="22" t="s">
-        <v>78</v>
-      </c>
+        <v>4111</v>
+      </c>
+      <c r="G33" s="20"/>
       <c r="H33" s="22"/>
-      <c r="I33" s="22">
-        <v>1</v>
-      </c>
-      <c r="J33" s="21"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="20"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
-    </row>
-    <row r="34" spans="1:16" ht="18">
+    </row>
+    <row r="34" spans="1:15" ht="18">
       <c r="A34" s="20" t="s">
         <v>103</v>
       </c>
       <c r="B34" s="20">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>189</v>
+        <v>107</v>
       </c>
       <c r="D34" s="20">
-        <v>99842</v>
+        <v>99898</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
       <c r="F34" s="20">
         <v>919</v>
@@ -10152,32 +10147,31 @@
       <c r="G34" s="20"/>
       <c r="H34" s="22"/>
       <c r="I34" s="22"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="22"/>
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-    </row>
-    <row r="35" spans="1:16" ht="18">
+    </row>
+    <row r="35" spans="1:15" ht="18">
       <c r="A35" s="20" t="s">
         <v>104</v>
       </c>
       <c r="B35" s="20">
-        <v>2899</v>
+        <v>2342</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D35" s="20">
-        <v>424507</v>
+        <v>425891</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="F35" s="20">
-        <v>7670</v>
+        <v>7679</v>
       </c>
       <c r="G35" s="22" t="s">
         <v>78</v>
@@ -10186,83 +10180,76 @@
       <c r="I35" s="22">
         <v>1</v>
       </c>
-      <c r="J35" s="21"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-    </row>
-    <row r="36" spans="1:16" ht="18">
+    </row>
+    <row r="36" spans="1:15" ht="18">
       <c r="A36" s="20" t="s">
         <v>105</v>
       </c>
       <c r="B36" s="20">
-        <v>7552</v>
+        <v>4409</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="D36" s="20">
-        <v>2032899</v>
+        <v>2038979</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="F36" s="20">
-        <v>23426</v>
+        <v>23447</v>
       </c>
       <c r="G36" s="22" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="H36" s="22"/>
       <c r="I36" s="22">
-        <v>2</v>
-      </c>
-      <c r="J36" s="21"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="J36" s="20"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="22"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
-      <c r="P36" s="22"/>
-    </row>
-    <row r="37" spans="1:16" ht="18">
+    </row>
+    <row r="37" spans="1:15" ht="18">
       <c r="A37" s="20" t="s">
         <v>106</v>
       </c>
       <c r="B37" s="20">
-        <v>6648</v>
+        <v>1988</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>132</v>
+        <v>208</v>
       </c>
       <c r="D37" s="20">
-        <v>1985308</v>
+        <v>1991410</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="F37" s="20">
-        <v>21119</v>
-      </c>
-      <c r="G37" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22">
-        <v>12</v>
-      </c>
-      <c r="J37" s="21"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="20"/>
+        <v>21169</v>
+      </c>
+      <c r="G37" s="22">
+        <v>4</v>
+      </c>
+      <c r="J37" s="20"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
-      <c r="P37" s="22"/>
-    </row>
-    <row r="38" spans="1:16" ht="18">
+    </row>
+    <row r="38" spans="1:15" ht="18">
       <c r="A38" s="20"/>
       <c r="B38" s="21"/>
       <c r="C38" s="20"/>
@@ -10281,8 +10268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C1D317E-D501-B04E-B622-A50394A159C7}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10312,13 +10299,13 @@
         <v>417036</v>
       </c>
       <c r="C2">
-        <v>328402</v>
+        <v>328563</v>
       </c>
       <c r="D2">
-        <v>319667</v>
+        <v>320674</v>
       </c>
       <c r="E2">
-        <v>8416</v>
+        <v>8805</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10329,13 +10316,13 @@
         <v>53903393</v>
       </c>
       <c r="C3">
-        <v>43029208</v>
+        <v>43051164</v>
       </c>
       <c r="D3">
-        <v>39989064</v>
+        <v>41017511</v>
       </c>
       <c r="E3">
-        <v>1303308</v>
+        <v>1398202</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -10346,13 +10333,13 @@
         <v>1570458</v>
       </c>
       <c r="C4">
-        <v>885898</v>
+        <v>887982</v>
       </c>
       <c r="D4">
-        <v>712899</v>
+        <v>721481</v>
       </c>
       <c r="E4">
-        <v>22460</v>
+        <v>23408</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -10363,13 +10350,13 @@
         <v>35607039</v>
       </c>
       <c r="C5">
-        <v>23348874</v>
+        <v>23383888</v>
       </c>
       <c r="D5">
-        <v>19367546</v>
+        <v>19611429</v>
       </c>
       <c r="E5">
-        <v>239362</v>
+        <v>256596</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -10380,13 +10367,13 @@
         <v>124799926</v>
       </c>
       <c r="C6">
-        <v>65970108</v>
+        <v>66316530</v>
       </c>
       <c r="D6">
-        <v>51310816</v>
+        <v>52622510</v>
       </c>
       <c r="E6">
-        <v>705256</v>
+        <v>766921</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -10397,13 +10384,13 @@
         <v>1158473</v>
       </c>
       <c r="C7">
-        <v>1121942</v>
+        <v>1123491</v>
       </c>
       <c r="D7">
-        <v>879319</v>
+        <v>885590</v>
       </c>
       <c r="E7">
-        <v>23338</v>
+        <v>24221</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -10414,13 +10401,13 @@
         <v>29436231</v>
       </c>
       <c r="C8">
-        <v>19586061</v>
+        <v>19638135</v>
       </c>
       <c r="D8">
-        <v>16274229</v>
+        <v>16649059</v>
       </c>
       <c r="E8">
-        <v>352101</v>
+        <v>371352</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -10431,13 +10418,13 @@
         <v>18710922</v>
       </c>
       <c r="C9">
-        <v>17241787</v>
+        <v>17284940</v>
       </c>
       <c r="D9">
-        <v>13354018</v>
+        <v>13640600</v>
       </c>
       <c r="E9">
-        <v>393760</v>
+        <v>414023</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -10448,13 +10435,13 @@
         <v>1586250</v>
       </c>
       <c r="C10">
-        <v>1390736</v>
+        <v>1391818</v>
       </c>
       <c r="D10">
-        <v>1218168</v>
+        <v>1221946</v>
       </c>
       <c r="E10">
-        <v>29501</v>
+        <v>30374</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -10465,13 +10452,13 @@
         <v>63872399</v>
       </c>
       <c r="C11">
-        <v>51886238</v>
+        <v>51999238</v>
       </c>
       <c r="D11">
-        <v>48221103</v>
+        <v>48866166</v>
       </c>
       <c r="E11">
-        <v>1948722</v>
+        <v>2037737</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -10482,13 +10469,13 @@
         <v>28204692</v>
       </c>
       <c r="C12">
-        <v>22804990</v>
+        <v>22850521</v>
       </c>
       <c r="D12">
-        <v>17764307</v>
+        <v>18006891</v>
       </c>
       <c r="E12">
-        <v>222613</v>
+        <v>235826</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -10499,13 +10486,13 @@
         <v>7451955</v>
       </c>
       <c r="C13">
-        <v>6315079</v>
+        <v>6320125</v>
       </c>
       <c r="D13">
-        <v>5892298</v>
+        <v>5913246</v>
       </c>
       <c r="E13">
-        <v>160803</v>
+        <v>173099</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -10516,13 +10503,13 @@
         <v>13606320</v>
       </c>
       <c r="C14">
-        <v>10714843</v>
+        <v>10736802</v>
       </c>
       <c r="D14">
-        <v>10361103</v>
+        <v>10470467</v>
       </c>
       <c r="E14">
-        <v>268611</v>
+        <v>285135</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -10533,13 +10520,13 @@
         <v>38593948</v>
       </c>
       <c r="C15">
-        <v>22106217</v>
+        <v>22220908</v>
       </c>
       <c r="D15">
-        <v>14072194</v>
+        <v>14436923</v>
       </c>
       <c r="E15">
-        <v>210401</v>
+        <v>224039</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -10550,13 +10537,13 @@
         <v>67562686</v>
       </c>
       <c r="C16">
-        <v>52064680</v>
+        <v>52124388</v>
       </c>
       <c r="D16">
-        <v>46450437</v>
+        <v>47294362</v>
       </c>
       <c r="E16">
-        <v>1127049</v>
+        <v>1187509</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -10567,13 +10554,13 @@
         <v>35699443</v>
       </c>
       <c r="C17">
-        <v>28052858</v>
+        <v>28083232</v>
       </c>
       <c r="D17">
-        <v>23310241</v>
+        <v>23560868</v>
       </c>
       <c r="E17">
-        <v>878552</v>
+        <v>906700</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -10584,13 +10571,13 @@
         <v>299000</v>
       </c>
       <c r="C18">
-        <v>226875</v>
+        <v>227054</v>
       </c>
       <c r="D18">
-        <v>186400</v>
+        <v>187395</v>
       </c>
       <c r="E18">
-        <v>26863</v>
+        <v>28184</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -10601,13 +10588,13 @@
         <v>289023</v>
       </c>
       <c r="C19">
-        <v>59492</v>
+        <v>59498</v>
       </c>
       <c r="D19">
-        <v>56674</v>
+        <v>56976</v>
       </c>
       <c r="E19">
-        <v>2282</v>
+        <v>2440</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -10618,13 +10605,13 @@
         <v>85358965</v>
       </c>
       <c r="C20">
-        <v>57888619</v>
+        <v>57966198</v>
       </c>
       <c r="D20">
-        <v>54267288</v>
+        <v>54814161</v>
       </c>
       <c r="E20">
-        <v>861939</v>
+        <v>886310</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -10635,13 +10622,13 @@
         <v>123144223</v>
       </c>
       <c r="C21">
-        <v>87109254</v>
+        <v>87328140</v>
       </c>
       <c r="D21">
-        <v>65174967</v>
+        <v>66728278</v>
       </c>
       <c r="E21">
-        <v>1431340</v>
+        <v>1513620</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -10652,13 +10639,13 @@
         <v>3091545</v>
       </c>
       <c r="C22">
-        <v>1498474</v>
+        <v>1510095</v>
       </c>
       <c r="D22">
-        <v>1113681</v>
+        <v>1136387</v>
       </c>
       <c r="E22">
-        <v>55535</v>
+        <v>59085</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -10669,13 +10656,13 @@
         <v>3366710</v>
       </c>
       <c r="C23">
-        <v>1355779</v>
+        <v>1359667</v>
       </c>
       <c r="D23">
-        <v>956468</v>
+        <v>965534</v>
       </c>
       <c r="E23">
-        <v>25655</v>
+        <v>26993</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -10686,13 +10673,13 @@
         <v>1239244</v>
       </c>
       <c r="C24">
-        <v>821318</v>
+        <v>823758</v>
       </c>
       <c r="D24">
-        <v>640411</v>
+        <v>648311</v>
       </c>
       <c r="E24">
-        <v>23625</v>
+        <v>24401</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -10703,13 +10690,13 @@
         <v>2249695</v>
       </c>
       <c r="C25">
-        <v>865077</v>
+        <v>870563</v>
       </c>
       <c r="D25">
-        <v>634442</v>
+        <v>647398</v>
       </c>
       <c r="E25">
-        <v>19629</v>
+        <v>21143</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -10720,13 +10707,13 @@
         <v>46356334</v>
       </c>
       <c r="C26">
-        <v>32633322</v>
+        <v>32747905</v>
       </c>
       <c r="D26">
-        <v>26824890</v>
+        <v>27398726</v>
       </c>
       <c r="E26">
-        <v>770777</v>
+        <v>799108</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -10737,13 +10724,13 @@
         <v>1413542</v>
       </c>
       <c r="C27">
-        <v>928494</v>
+        <v>931304</v>
       </c>
       <c r="D27">
-        <v>629283</v>
+        <v>646844</v>
       </c>
       <c r="E27">
-        <v>11955</v>
+        <v>12368</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -10754,13 +10741,13 @@
         <v>30141373</v>
       </c>
       <c r="C28">
-        <v>22334192</v>
+        <v>22512581</v>
       </c>
       <c r="D28">
-        <v>15873590</v>
+        <v>16152325</v>
       </c>
       <c r="E28">
-        <v>379135</v>
+        <v>393361</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -10771,13 +10758,13 @@
         <v>81032689</v>
       </c>
       <c r="C29">
-        <v>53587710</v>
+        <v>53785334</v>
       </c>
       <c r="D29">
-        <v>43049408</v>
+        <v>43676509</v>
       </c>
       <c r="E29">
-        <v>1211849</v>
+        <v>1277366</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -10788,13 +10775,13 @@
         <v>690251</v>
       </c>
       <c r="C30">
-        <v>562464</v>
+        <v>563106</v>
       </c>
       <c r="D30">
-        <v>510476</v>
+        <v>514824</v>
       </c>
       <c r="E30">
-        <v>28248</v>
+        <v>29385</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -10805,13 +10792,13 @@
         <v>77841267</v>
       </c>
       <c r="C31">
-        <v>55545388</v>
+        <v>55700626</v>
       </c>
       <c r="D31">
-        <v>41443382</v>
+        <v>42140120</v>
       </c>
       <c r="E31">
-        <v>544242</v>
+        <v>568783</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -10822,13 +10809,13 @@
         <v>38510982</v>
       </c>
       <c r="C32">
-        <v>30798908</v>
+        <v>30874859</v>
       </c>
       <c r="D32">
-        <v>26407374</v>
+        <v>26953746</v>
       </c>
       <c r="E32">
-        <v>433473</v>
+        <v>467657</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -10839,13 +10826,13 @@
         <v>4169794</v>
       </c>
       <c r="C33">
-        <v>2763180</v>
+        <v>2765407</v>
       </c>
       <c r="D33">
-        <v>2265805</v>
+        <v>2278690</v>
       </c>
       <c r="E33">
-        <v>62102</v>
+        <v>65166</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -10856,13 +10843,13 @@
         <v>237882725</v>
       </c>
       <c r="C34">
-        <v>163687535</v>
+        <v>164534086</v>
       </c>
       <c r="D34">
-        <v>116638430</v>
+        <v>121008880</v>
       </c>
       <c r="E34">
-        <v>2156451</v>
+        <v>2247713</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -10873,13 +10860,13 @@
         <v>11250858</v>
       </c>
       <c r="C35">
-        <v>8556611</v>
+        <v>8570163</v>
       </c>
       <c r="D35">
-        <v>7835777</v>
+        <v>7892108</v>
       </c>
       <c r="E35">
-        <v>377317</v>
+        <v>392757</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -10890,13 +10877,13 @@
         <v>99609303</v>
       </c>
       <c r="C36">
-        <v>69919065</v>
+        <v>70037735</v>
       </c>
       <c r="D36">
-        <v>57763823</v>
+        <v>59142774</v>
       </c>
       <c r="E36">
-        <v>1553629</v>
+        <v>1638983</v>
       </c>
     </row>
   </sheetData>
@@ -10906,10 +10893,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCA94CA-D9DE-B548-8735-C3641B00F463}">
-  <dimension ref="A1:S323"/>
+  <dimension ref="A1:S329"/>
   <sheetViews>
-    <sheetView topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="D319" sqref="D319"/>
+    <sheetView topLeftCell="A313" workbookViewId="0">
+      <selection activeCell="D329" sqref="D329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -29968,6 +29955,360 @@
         <v>64000</v>
       </c>
       <c r="S323" s="17">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="324" spans="1:19">
+      <c r="A324" s="3">
+        <v>44613</v>
+      </c>
+      <c r="B324" s="17">
+        <v>22000</v>
+      </c>
+      <c r="C324" s="17">
+        <v>21500</v>
+      </c>
+      <c r="D324" s="17">
+        <v>12500</v>
+      </c>
+      <c r="E324" s="17">
+        <v>35000</v>
+      </c>
+      <c r="F324" s="17">
+        <v>28500</v>
+      </c>
+      <c r="G324" s="17">
+        <v>32000</v>
+      </c>
+      <c r="H324" s="17">
+        <v>18500</v>
+      </c>
+      <c r="I324" s="17">
+        <v>20500</v>
+      </c>
+      <c r="J324" s="17">
+        <v>31500</v>
+      </c>
+      <c r="K324" s="17">
+        <v>31500</v>
+      </c>
+      <c r="L324" s="17">
+        <v>50000</v>
+      </c>
+      <c r="M324" s="17">
+        <v>82000</v>
+      </c>
+      <c r="N324" s="17">
+        <v>63000</v>
+      </c>
+      <c r="O324" s="17">
+        <v>84500</v>
+      </c>
+      <c r="P324" s="17">
+        <v>88000</v>
+      </c>
+      <c r="Q324" s="17">
+        <v>89000</v>
+      </c>
+      <c r="R324" s="17">
+        <v>64000</v>
+      </c>
+      <c r="S324" s="17">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="325" spans="1:19">
+      <c r="A325" s="3">
+        <v>44614</v>
+      </c>
+      <c r="B325" s="17">
+        <v>22000</v>
+      </c>
+      <c r="C325" s="17">
+        <v>21500</v>
+      </c>
+      <c r="D325" s="17">
+        <v>12500</v>
+      </c>
+      <c r="E325" s="17">
+        <v>35000</v>
+      </c>
+      <c r="F325" s="17">
+        <v>28500</v>
+      </c>
+      <c r="G325" s="17">
+        <v>32000</v>
+      </c>
+      <c r="H325" s="17">
+        <v>18500</v>
+      </c>
+      <c r="I325" s="17">
+        <v>20500</v>
+      </c>
+      <c r="J325" s="17">
+        <v>31500</v>
+      </c>
+      <c r="K325" s="17">
+        <v>31500</v>
+      </c>
+      <c r="L325" s="17">
+        <v>50000</v>
+      </c>
+      <c r="M325" s="17">
+        <v>82000</v>
+      </c>
+      <c r="N325" s="17">
+        <v>63000</v>
+      </c>
+      <c r="O325" s="17">
+        <v>84500</v>
+      </c>
+      <c r="P325" s="17">
+        <v>88000</v>
+      </c>
+      <c r="Q325" s="17">
+        <v>89000</v>
+      </c>
+      <c r="R325" s="17">
+        <v>64000</v>
+      </c>
+      <c r="S325" s="17">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="326" spans="1:19">
+      <c r="A326" s="3">
+        <v>44615</v>
+      </c>
+      <c r="B326" s="17">
+        <v>22000</v>
+      </c>
+      <c r="C326" s="17">
+        <v>21500</v>
+      </c>
+      <c r="D326" s="17">
+        <v>12500</v>
+      </c>
+      <c r="E326" s="17">
+        <v>35000</v>
+      </c>
+      <c r="F326" s="17">
+        <v>28500</v>
+      </c>
+      <c r="G326" s="17">
+        <v>32000</v>
+      </c>
+      <c r="H326" s="17">
+        <v>18500</v>
+      </c>
+      <c r="I326" s="17">
+        <v>20500</v>
+      </c>
+      <c r="J326" s="17">
+        <v>31500</v>
+      </c>
+      <c r="K326" s="17">
+        <v>31500</v>
+      </c>
+      <c r="L326" s="17">
+        <v>50000</v>
+      </c>
+      <c r="M326" s="17">
+        <v>82000</v>
+      </c>
+      <c r="N326" s="17">
+        <v>63000</v>
+      </c>
+      <c r="O326" s="17">
+        <v>84500</v>
+      </c>
+      <c r="P326" s="17">
+        <v>88000</v>
+      </c>
+      <c r="Q326" s="17">
+        <v>89000</v>
+      </c>
+      <c r="R326" s="17">
+        <v>64000</v>
+      </c>
+      <c r="S326" s="17">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="327" spans="1:19">
+      <c r="A327" s="3">
+        <v>44616</v>
+      </c>
+      <c r="B327" s="17">
+        <v>22000</v>
+      </c>
+      <c r="C327" s="17">
+        <v>21500</v>
+      </c>
+      <c r="D327" s="17">
+        <v>12500</v>
+      </c>
+      <c r="E327" s="17">
+        <v>35000</v>
+      </c>
+      <c r="F327" s="17">
+        <v>28500</v>
+      </c>
+      <c r="G327" s="17">
+        <v>32000</v>
+      </c>
+      <c r="H327" s="17">
+        <v>18500</v>
+      </c>
+      <c r="I327" s="17">
+        <v>20500</v>
+      </c>
+      <c r="J327" s="17">
+        <v>31500</v>
+      </c>
+      <c r="K327" s="17">
+        <v>31500</v>
+      </c>
+      <c r="L327" s="17">
+        <v>50000</v>
+      </c>
+      <c r="M327" s="17">
+        <v>82000</v>
+      </c>
+      <c r="N327" s="17">
+        <v>63000</v>
+      </c>
+      <c r="O327" s="17">
+        <v>84500</v>
+      </c>
+      <c r="P327" s="17">
+        <v>88000</v>
+      </c>
+      <c r="Q327" s="17">
+        <v>89000</v>
+      </c>
+      <c r="R327" s="17">
+        <v>64000</v>
+      </c>
+      <c r="S327" s="17">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="328" spans="1:19">
+      <c r="A328" s="3">
+        <v>44617</v>
+      </c>
+      <c r="B328" s="17">
+        <v>22000</v>
+      </c>
+      <c r="C328" s="17">
+        <v>21500</v>
+      </c>
+      <c r="D328" s="17">
+        <v>12500</v>
+      </c>
+      <c r="E328" s="17">
+        <v>35000</v>
+      </c>
+      <c r="F328" s="17">
+        <v>28500</v>
+      </c>
+      <c r="G328" s="17">
+        <v>32000</v>
+      </c>
+      <c r="H328" s="17">
+        <v>18500</v>
+      </c>
+      <c r="I328" s="17">
+        <v>20500</v>
+      </c>
+      <c r="J328" s="17">
+        <v>31500</v>
+      </c>
+      <c r="K328" s="17">
+        <v>31500</v>
+      </c>
+      <c r="L328" s="17">
+        <v>50000</v>
+      </c>
+      <c r="M328" s="17">
+        <v>82000</v>
+      </c>
+      <c r="N328" s="17">
+        <v>63000</v>
+      </c>
+      <c r="O328" s="17">
+        <v>84500</v>
+      </c>
+      <c r="P328" s="17">
+        <v>88000</v>
+      </c>
+      <c r="Q328" s="17">
+        <v>89000</v>
+      </c>
+      <c r="R328" s="17">
+        <v>64000</v>
+      </c>
+      <c r="S328" s="17">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="329" spans="1:19">
+      <c r="A329" s="3">
+        <v>44618</v>
+      </c>
+      <c r="B329" s="17">
+        <v>22000</v>
+      </c>
+      <c r="C329" s="17">
+        <v>21500</v>
+      </c>
+      <c r="D329" s="17">
+        <v>12500</v>
+      </c>
+      <c r="E329" s="17">
+        <v>35000</v>
+      </c>
+      <c r="F329" s="17">
+        <v>28500</v>
+      </c>
+      <c r="G329" s="17">
+        <v>32000</v>
+      </c>
+      <c r="H329" s="17">
+        <v>18500</v>
+      </c>
+      <c r="I329" s="17">
+        <v>20500</v>
+      </c>
+      <c r="J329" s="17">
+        <v>31500</v>
+      </c>
+      <c r="K329" s="17">
+        <v>31500</v>
+      </c>
+      <c r="L329" s="17">
+        <v>50000</v>
+      </c>
+      <c r="M329" s="17">
+        <v>82000</v>
+      </c>
+      <c r="N329" s="17">
+        <v>63000</v>
+      </c>
+      <c r="O329" s="17">
+        <v>84500</v>
+      </c>
+      <c r="P329" s="17">
+        <v>88000</v>
+      </c>
+      <c r="Q329" s="17">
+        <v>89000</v>
+      </c>
+      <c r="R329" s="17">
+        <v>64000</v>
+      </c>
+      <c r="S329" s="17">
         <v>52000</v>
       </c>
     </row>
@@ -29980,8 +30321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8984DF-48CB-5447-B9FA-A4B1DAFD9CF3}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30008,39 +30349,39 @@
       <c r="A2" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B2" s="27">
-        <v>10400661</v>
-      </c>
-      <c r="C2" s="27">
-        <v>9952131</v>
-      </c>
-      <c r="D2" s="27">
-        <v>4045802</v>
+      <c r="B2" s="36">
+        <v>10401480</v>
+      </c>
+      <c r="C2" s="36">
+        <v>9965907</v>
+      </c>
+      <c r="D2" s="36">
+        <v>4166909</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20">
       <c r="A3" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="27">
-        <v>18407876</v>
-      </c>
-      <c r="C3" s="27">
-        <v>17415830</v>
-      </c>
-      <c r="D3" s="27">
-        <v>5897178</v>
+      <c r="B3" s="36">
+        <v>18409341</v>
+      </c>
+      <c r="C3" s="36">
+        <v>17439847</v>
+      </c>
+      <c r="D3" s="36">
+        <v>6191330</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20">
       <c r="A4" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B4" s="27">
-        <v>53625069</v>
-      </c>
-      <c r="C4" s="27">
-        <v>21557154</v>
+      <c r="B4" s="36">
+        <v>54747973</v>
+      </c>
+      <c r="C4" s="36">
+        <v>27260355</v>
       </c>
       <c r="D4" s="19"/>
     </row>
@@ -30048,11 +30389,11 @@
       <c r="A5" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="27">
-        <v>550294446</v>
-      </c>
-      <c r="C5" s="27">
-        <v>435543092</v>
+      <c r="B5" s="36">
+        <v>551674510</v>
+      </c>
+      <c r="C5" s="36">
+        <v>443457581</v>
       </c>
       <c r="D5" s="19"/>
     </row>
@@ -30060,11 +30401,11 @@
       <c r="A6" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="27">
-        <v>202030925</v>
-      </c>
-      <c r="C6" s="27">
-        <v>178284433</v>
+      <c r="B6" s="36">
+        <v>202251597</v>
+      </c>
+      <c r="C6" s="36">
+        <v>179982110</v>
       </c>
       <c r="D6" s="19"/>
     </row>
@@ -30072,14 +30413,14 @@
       <c r="A7" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="27">
-        <v>126199513</v>
-      </c>
-      <c r="C7" s="27">
-        <v>111065151</v>
-      </c>
-      <c r="D7" s="27">
-        <v>9003436</v>
+      <c r="B7" s="36">
+        <v>126392536</v>
+      </c>
+      <c r="C7" s="36">
+        <v>112113754</v>
+      </c>
+      <c r="D7" s="36">
+        <v>9604490</v>
       </c>
     </row>
   </sheetData>
@@ -30089,10 +30430,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5A5412-72F4-CA4E-9682-44F6B6C554A4}">
-  <dimension ref="A1:B1147"/>
+  <dimension ref="A1:B1153"/>
   <sheetViews>
-    <sheetView topLeftCell="A1138" workbookViewId="0">
-      <selection activeCell="A1138" sqref="A1138"/>
+    <sheetView topLeftCell="A1144" workbookViewId="0">
+      <selection activeCell="A1153" sqref="A1153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -39273,6 +39614,54 @@
         <v>3948</v>
       </c>
     </row>
+    <row r="1148" spans="1:2">
+      <c r="A1148" s="4">
+        <v>44612</v>
+      </c>
+      <c r="B1148">
+        <v>3902</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:2">
+      <c r="A1149" s="4">
+        <v>44613</v>
+      </c>
+      <c r="B1149">
+        <v>3936</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:2">
+      <c r="A1150" s="4">
+        <v>44614</v>
+      </c>
+      <c r="B1150">
+        <v>4003</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:2">
+      <c r="A1151" s="4">
+        <v>44615</v>
+      </c>
+      <c r="B1151">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:2">
+      <c r="A1152" s="4">
+        <v>44616</v>
+      </c>
+      <c r="B1152">
+        <v>4041</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:2">
+      <c r="A1153" s="4">
+        <v>44617</v>
+      </c>
+      <c r="B1153">
+        <v>4042</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -39280,10 +39669,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44E43D3-B2B8-4440-9DFA-30FE18FECCE6}">
-  <dimension ref="A1:B629"/>
+  <dimension ref="A1:B636"/>
   <sheetViews>
-    <sheetView topLeftCell="A614" workbookViewId="0">
-      <selection activeCell="A629" sqref="A629"/>
+    <sheetView topLeftCell="A620" workbookViewId="0">
+      <selection activeCell="B629" sqref="B629"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -44320,6 +44709,62 @@
         <v>27226.799999999999</v>
       </c>
     </row>
+    <row r="630" spans="1:2">
+      <c r="A630" s="4">
+        <v>44611</v>
+      </c>
+      <c r="B630" s="18">
+        <v>25778.25</v>
+      </c>
+    </row>
+    <row r="631" spans="1:2">
+      <c r="A631" s="4">
+        <v>44612</v>
+      </c>
+      <c r="B631" s="18">
+        <v>21128.33</v>
+      </c>
+    </row>
+    <row r="632" spans="1:2">
+      <c r="A632" s="4">
+        <v>44613</v>
+      </c>
+      <c r="B632" s="18">
+        <v>29480.41</v>
+      </c>
+    </row>
+    <row r="633" spans="1:2">
+      <c r="A633" s="4">
+        <v>44614</v>
+      </c>
+      <c r="B633" s="18">
+        <v>27023.99</v>
+      </c>
+    </row>
+    <row r="634" spans="1:2">
+      <c r="A634" s="4">
+        <v>44615</v>
+      </c>
+      <c r="B634" s="18">
+        <v>24444.21</v>
+      </c>
+    </row>
+    <row r="635" spans="1:2">
+      <c r="A635" s="4">
+        <v>44616</v>
+      </c>
+      <c r="B635" s="18">
+        <v>32003.16</v>
+      </c>
+    </row>
+    <row r="636" spans="1:2">
+      <c r="A636" s="4">
+        <v>44617</v>
+      </c>
+      <c r="B636" s="18">
+        <v>29271.51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44327,10 +44772,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D064278-E4AD-8149-B400-6EAC50E0DC3D}">
-  <dimension ref="A1:B553"/>
+  <dimension ref="A1:B559"/>
   <sheetViews>
-    <sheetView topLeftCell="A542" zoomScale="132" workbookViewId="0">
-      <selection activeCell="A553" sqref="A553"/>
+    <sheetView topLeftCell="A548" zoomScale="132" workbookViewId="0">
+      <selection activeCell="A559" sqref="A559"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -48759,6 +49204,54 @@
         <v>7.63</v>
       </c>
     </row>
+    <row r="554" spans="1:2">
+      <c r="A554" s="3">
+        <v>44612</v>
+      </c>
+      <c r="B554">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="555" spans="1:2">
+      <c r="A555" s="3">
+        <v>44613</v>
+      </c>
+      <c r="B555">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="556" spans="1:2">
+      <c r="A556" s="3">
+        <v>44614</v>
+      </c>
+      <c r="B556">
+        <v>8.06</v>
+      </c>
+    </row>
+    <row r="557" spans="1:2">
+      <c r="A557" s="3">
+        <v>44615</v>
+      </c>
+      <c r="B557">
+        <v>8.23</v>
+      </c>
+    </row>
+    <row r="558" spans="1:2">
+      <c r="A558" s="3">
+        <v>44616</v>
+      </c>
+      <c r="B558">
+        <v>8.11</v>
+      </c>
+    </row>
+    <row r="559" spans="1:2">
+      <c r="A559" s="3">
+        <v>44617</v>
+      </c>
+      <c r="B559">
+        <v>8.15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -48766,290 +49259,464 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70EF183-B223-BA44-B3E0-EC1BFDE7C01F}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="D1" s="28" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="B2" s="30">
-        <v>-0.17735211707621867</v>
-      </c>
-      <c r="C2" s="30">
-        <v>-0.45864832389983623</v>
-      </c>
-      <c r="D2" s="30">
-        <v>-0.39957622427515282</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="B3" s="30">
-        <v>-0.42169635735176814</v>
-      </c>
-      <c r="C3" s="30">
-        <v>-0.52364393813460708</v>
-      </c>
-      <c r="D3" s="30">
-        <v>-0.46022632568229782</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="B4" s="30">
-        <v>0.16097513622109383</v>
-      </c>
-      <c r="C4" s="30">
-        <v>-0.19143531974841188</v>
-      </c>
-      <c r="D4" s="30">
-        <v>-5.65070900496909E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="30">
-        <v>-2.0152972166682548E-2</v>
-      </c>
-      <c r="C5" s="30">
-        <v>-0.33197530104416684</v>
-      </c>
-      <c r="D5" s="30">
-        <v>-0.22569103580324035</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" s="30">
-        <v>-0.16588285745706499</v>
-      </c>
-      <c r="C6" s="30">
-        <v>-0.31981553451902034</v>
-      </c>
-      <c r="D6" s="30">
-        <v>-0.20896245562648241</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="29" t="s">
-        <v>203</v>
-      </c>
-      <c r="B7" s="30">
-        <v>-0.17415571610611713</v>
-      </c>
-      <c r="C7" s="30">
-        <v>-0.17664582429181463</v>
-      </c>
-      <c r="D7" s="30">
-        <v>-0.17544644096981143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="29" t="s">
-        <v>204</v>
-      </c>
-      <c r="B8" s="30">
-        <v>-0.25518182243006426</v>
-      </c>
-      <c r="C8" s="30">
-        <v>-0.81865645467779558</v>
-      </c>
-      <c r="D8" s="30">
-        <v>-0.4960698868526574</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="29" t="s">
-        <v>205</v>
-      </c>
-      <c r="B9" s="30">
-        <v>-6.9279233739349966E-3</v>
-      </c>
-      <c r="C9" s="30">
-        <v>-0.86681022282244224</v>
-      </c>
-      <c r="D9" s="30">
-        <v>-0.21913867185817815</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="29" t="s">
-        <v>206</v>
-      </c>
-      <c r="B10" s="30">
-        <v>-0.36550769915729397</v>
-      </c>
-      <c r="C10" s="30">
-        <v>-0.45605680743869892</v>
-      </c>
-      <c r="D10" s="30">
-        <v>-0.42873704245052968</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="B11" s="30">
-        <v>3.7593456359970467E-2</v>
-      </c>
-      <c r="C11" s="30">
-        <v>-0.3948121358113309</v>
-      </c>
-      <c r="D11" s="30">
-        <v>-0.25060548738908706</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="B12" s="30">
-        <v>-0.29843049032376889</v>
-      </c>
-      <c r="C12" s="30">
-        <v>-0.19965577917079069</v>
-      </c>
-      <c r="D12" s="30">
-        <v>-0.20727567235116628</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="29" t="s">
-        <v>209</v>
-      </c>
-      <c r="B13" s="30">
-        <v>5.6759953977539634E-2</v>
-      </c>
-      <c r="C13" s="30">
-        <v>-5.3973991489100426E-2</v>
-      </c>
-      <c r="D13" s="30">
-        <v>6.0563786123917218E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="B14" s="30">
-        <v>1.9534758774691241E-2</v>
-      </c>
-      <c r="C14" s="30">
-        <v>-0.31088734516914962</v>
-      </c>
-      <c r="D14" s="30">
-        <v>-7.3827762924827289E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="29" t="s">
-        <v>211</v>
-      </c>
-      <c r="B15" s="30">
-        <v>-0.19580412633079769</v>
-      </c>
-      <c r="C15" s="30">
-        <v>-0.53495480825990149</v>
-      </c>
-      <c r="D15" s="30">
-        <v>-0.25830707577622791</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="B16" s="30">
-        <v>-0.16298906869037799</v>
-      </c>
-      <c r="C16" s="30">
-        <v>-0.30202906701789001</v>
-      </c>
-      <c r="D16" s="30">
-        <v>-0.2698307763711586</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="29" t="s">
-        <v>213</v>
-      </c>
-      <c r="B17" s="30">
-        <v>-7.921595910553747E-2</v>
-      </c>
-      <c r="C17" s="30">
-        <v>-0.31775758817335953</v>
-      </c>
-      <c r="D17" s="30">
-        <v>-0.1176482619802941</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="29" t="s">
-        <v>214</v>
-      </c>
-      <c r="B18" s="30">
-        <v>-0.25451552902388619</v>
-      </c>
-      <c r="C18" s="30">
-        <v>-0.78124789408620743</v>
-      </c>
-      <c r="D18" s="30">
-        <v>-0.42220330077296586</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="B19" s="30">
-        <v>-0.11381232163002042</v>
-      </c>
-      <c r="C19" s="30">
-        <v>-0.50500126046625582</v>
-      </c>
-      <c r="D19" s="30">
-        <v>-0.26737909949125938</v>
-      </c>
+    <row r="1" spans="1:6">
+      <c r="A1" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18">
+      <c r="A2" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="35">
+        <v>-6.0999999999999999E-2</v>
+      </c>
+      <c r="C2" s="35">
+        <v>-0.22700000000000001</v>
+      </c>
+      <c r="D2" s="35">
+        <v>-0.193</v>
+      </c>
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="1:6" ht="18">
+      <c r="A3" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="35">
+        <v>-0.372</v>
+      </c>
+      <c r="C3" s="35">
+        <v>-0.46500000000000002</v>
+      </c>
+      <c r="D3" s="35">
+        <v>-0.40600000000000003</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:6" ht="18">
+      <c r="A4" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="35">
+        <v>0.437</v>
+      </c>
+      <c r="C4" s="35">
+        <v>-0.151</v>
+      </c>
+      <c r="D4" s="35">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:6" ht="18">
+      <c r="A5" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="35">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C5" s="35">
+        <v>-0.30199999999999999</v>
+      </c>
+      <c r="D5" s="35">
+        <v>-0.19900000000000001</v>
+      </c>
+      <c r="E5" s="32"/>
+      <c r="F5" s="31"/>
+    </row>
+    <row r="6" spans="1:6" ht="18">
+      <c r="A6" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="35">
+        <v>-6.6000000000000003E-2</v>
+      </c>
+      <c r="C6" s="35">
+        <v>-0.32900000000000001</v>
+      </c>
+      <c r="D6" s="35">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="1:6" ht="18">
+      <c r="A7" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="35">
+        <v>-0.161</v>
+      </c>
+      <c r="C7" s="35">
+        <v>-9.7000000000000003E-2</v>
+      </c>
+      <c r="D7" s="35">
+        <v>-0.128</v>
+      </c>
+      <c r="F7" s="31"/>
+    </row>
+    <row r="8" spans="1:6" ht="18">
+      <c r="A8" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="35">
+        <v>-0.24099999999999999</v>
+      </c>
+      <c r="C8" s="35">
+        <v>-0.81499999999999995</v>
+      </c>
+      <c r="D8" s="35">
+        <v>-0.48499999999999999</v>
+      </c>
+      <c r="F8" s="31"/>
+    </row>
+    <row r="9" spans="1:6" ht="18">
+      <c r="A9" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="35">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C9" s="35">
+        <v>-0.86599999999999999</v>
+      </c>
+      <c r="D9" s="35">
+        <v>-0.20799999999999999</v>
+      </c>
+      <c r="F9" s="31"/>
+    </row>
+    <row r="10" spans="1:6" ht="18">
+      <c r="A10" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="35">
+        <v>-0.29899999999999999</v>
+      </c>
+      <c r="C10" s="35">
+        <v>-0.33500000000000002</v>
+      </c>
+      <c r="D10" s="35">
+        <v>-0.32500000000000001</v>
+      </c>
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" spans="1:6" ht="18">
+      <c r="A11" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="35">
+        <v>0</v>
+      </c>
+      <c r="C11" s="35">
+        <v>-0.34200000000000003</v>
+      </c>
+      <c r="D11" s="35">
+        <v>-0.22800000000000001</v>
+      </c>
+      <c r="F11" s="31"/>
+    </row>
+    <row r="12" spans="1:6" ht="18">
+      <c r="A12" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="35">
+        <v>-0.29199999999999998</v>
+      </c>
+      <c r="C12" s="35">
+        <v>-0.183</v>
+      </c>
+      <c r="D12" s="35">
+        <v>-0.191</v>
+      </c>
+      <c r="F12" s="31"/>
+    </row>
+    <row r="13" spans="1:6" ht="18">
+      <c r="A13" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" s="35">
+        <v>-8.0000000000000002E-3</v>
+      </c>
+      <c r="C13" s="35">
+        <v>-4.8000000000000001E-2</v>
+      </c>
+      <c r="D13" s="35">
+        <v>-2.7E-2</v>
+      </c>
+      <c r="F13" s="31"/>
+    </row>
+    <row r="14" spans="1:6" ht="18">
+      <c r="A14" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="35">
+        <v>0.153</v>
+      </c>
+      <c r="C14" s="35">
+        <v>-0.27700000000000002</v>
+      </c>
+      <c r="D14" s="35">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F14" s="30"/>
+    </row>
+    <row r="15" spans="1:6" ht="18">
+      <c r="A15" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" s="35">
+        <v>-0.154</v>
+      </c>
+      <c r="C15" s="35">
+        <v>-0.47499999999999998</v>
+      </c>
+      <c r="D15" s="35">
+        <v>-0.214</v>
+      </c>
+      <c r="F15" s="31"/>
+    </row>
+    <row r="16" spans="1:6" ht="18">
+      <c r="A16" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" s="35">
+        <v>-0.16500000000000001</v>
+      </c>
+      <c r="C16" s="35">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="D16" s="35">
+        <v>-0.26200000000000001</v>
+      </c>
+      <c r="F16" s="31"/>
+    </row>
+    <row r="17" spans="1:6" ht="18">
+      <c r="A17" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="35">
+        <v>-7.4999999999999997E-2</v>
+      </c>
+      <c r="C17" s="35">
+        <v>-0.32900000000000001</v>
+      </c>
+      <c r="D17" s="35">
+        <v>-0.115</v>
+      </c>
+      <c r="F17" s="31"/>
+    </row>
+    <row r="18" spans="1:6" ht="18">
+      <c r="A18" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" s="35">
+        <v>-0.34100000000000003</v>
+      </c>
+      <c r="C18" s="35">
+        <v>-0.77800000000000002</v>
+      </c>
+      <c r="D18" s="35">
+        <v>-0.47</v>
+      </c>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="1:6" ht="18">
+      <c r="A19" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="35">
+        <v>-9.2999999999999999E-2</v>
+      </c>
+      <c r="C19" s="35">
+        <v>-0.45</v>
+      </c>
+      <c r="D19" s="35">
+        <v>-0.23499999999999999</v>
+      </c>
+      <c r="F19" s="31"/>
+    </row>
+    <row r="20" spans="1:6" ht="18">
+      <c r="F20" s="31"/>
+    </row>
+    <row r="21" spans="1:6" ht="18">
+      <c r="F21" s="31"/>
+    </row>
+    <row r="22" spans="1:6" ht="18">
+      <c r="F22" s="30"/>
+    </row>
+    <row r="23" spans="1:6" ht="18">
+      <c r="F23" s="31"/>
+    </row>
+    <row r="24" spans="1:6" ht="18">
+      <c r="F24" s="31"/>
+    </row>
+    <row r="25" spans="1:6" ht="18">
+      <c r="F25" s="31"/>
+    </row>
+    <row r="26" spans="1:6" ht="18">
+      <c r="F26" s="30"/>
+    </row>
+    <row r="27" spans="1:6" ht="18">
+      <c r="F27" s="31"/>
+    </row>
+    <row r="28" spans="1:6" ht="18">
+      <c r="F28" s="31"/>
+    </row>
+    <row r="29" spans="1:6" ht="18">
+      <c r="F29" s="31"/>
+    </row>
+    <row r="30" spans="1:6" ht="18">
+      <c r="F30" s="30"/>
+    </row>
+    <row r="31" spans="1:6" ht="18">
+      <c r="F31" s="31"/>
+    </row>
+    <row r="32" spans="1:6" ht="18">
+      <c r="F32" s="31"/>
+    </row>
+    <row r="33" spans="6:6" ht="18">
+      <c r="F33" s="31"/>
+    </row>
+    <row r="34" spans="6:6" ht="18">
+      <c r="F34" s="30"/>
+    </row>
+    <row r="35" spans="6:6" ht="18">
+      <c r="F35" s="31"/>
+    </row>
+    <row r="36" spans="6:6" ht="18">
+      <c r="F36" s="31"/>
+    </row>
+    <row r="37" spans="6:6" ht="18">
+      <c r="F37" s="31"/>
+    </row>
+    <row r="38" spans="6:6" ht="18">
+      <c r="F38" s="30"/>
+    </row>
+    <row r="39" spans="6:6" ht="18">
+      <c r="F39" s="31"/>
+    </row>
+    <row r="40" spans="6:6" ht="18">
+      <c r="F40" s="31"/>
+    </row>
+    <row r="41" spans="6:6" ht="18">
+      <c r="F41" s="31"/>
+    </row>
+    <row r="42" spans="6:6" ht="18">
+      <c r="F42" s="30"/>
+    </row>
+    <row r="43" spans="6:6" ht="18">
+      <c r="F43" s="31"/>
+    </row>
+    <row r="44" spans="6:6" ht="18">
+      <c r="F44" s="31"/>
+    </row>
+    <row r="45" spans="6:6" ht="18">
+      <c r="F45" s="31"/>
+    </row>
+    <row r="46" spans="6:6" ht="18">
+      <c r="F46" s="30"/>
+    </row>
+    <row r="47" spans="6:6" ht="18">
+      <c r="F47" s="31"/>
+    </row>
+    <row r="48" spans="6:6" ht="18">
+      <c r="F48" s="31"/>
+    </row>
+    <row r="49" spans="6:6" ht="18">
+      <c r="F49" s="31"/>
+    </row>
+    <row r="50" spans="6:6" ht="18">
+      <c r="F50" s="30"/>
+    </row>
+    <row r="51" spans="6:6" ht="18">
+      <c r="F51" s="31"/>
+    </row>
+    <row r="52" spans="6:6" ht="18">
+      <c r="F52" s="31"/>
+    </row>
+    <row r="53" spans="6:6" ht="18">
+      <c r="F53" s="31"/>
+    </row>
+    <row r="54" spans="6:6" ht="18">
+      <c r="F54" s="30"/>
+    </row>
+    <row r="55" spans="6:6" ht="18">
+      <c r="F55" s="31"/>
+    </row>
+    <row r="56" spans="6:6" ht="18">
+      <c r="F56" s="31"/>
+    </row>
+    <row r="57" spans="6:6" ht="18">
+      <c r="F57" s="31"/>
+    </row>
+    <row r="58" spans="6:6" ht="18">
+      <c r="F58" s="30"/>
+    </row>
+    <row r="59" spans="6:6" ht="18">
+      <c r="F59" s="31"/>
+    </row>
+    <row r="60" spans="6:6" ht="18">
+      <c r="F60" s="31"/>
+    </row>
+    <row r="61" spans="6:6" ht="18">
+      <c r="F61" s="31"/>
+    </row>
+    <row r="62" spans="6:6" ht="18">
+      <c r="F62" s="30"/>
+    </row>
+    <row r="63" spans="6:6" ht="18">
+      <c r="F63" s="31"/>
+    </row>
+    <row r="64" spans="6:6" ht="18">
+      <c r="F64" s="31"/>
+    </row>
+    <row r="65" spans="6:6" ht="18">
+      <c r="F65" s="31"/>
+    </row>
+    <row r="66" spans="6:6" ht="18">
+      <c r="F66" s="30"/>
+    </row>
+    <row r="67" spans="6:6" ht="18">
+      <c r="F67" s="31"/>
+    </row>
+    <row r="68" spans="6:6" ht="18">
+      <c r="F68" s="31"/>
+    </row>
+    <row r="69" spans="6:6" ht="18">
+      <c r="F69" s="31"/>
+    </row>
+    <row r="70" spans="6:6" ht="18">
+      <c r="F70" s="30"/>
+    </row>
+    <row r="71" spans="6:6" ht="18">
+      <c r="F71" s="31"/>
+    </row>
+    <row r="72" spans="6:6" ht="18">
+      <c r="F72" s="31"/>
+    </row>
+    <row r="73" spans="6:6" ht="18">
+      <c r="F73" s="31"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D19">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -49058,272 +49725,272 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288B73DA-0631-CA47-AE4E-9C96F2353AB8}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="28" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>196</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>197</v>
+      <c r="A1" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="29" t="s">
-        <v>198</v>
-      </c>
-      <c r="B2" s="30">
+      <c r="A2" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="29">
         <v>-9.8584166412597596E-2</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="29">
         <v>-8.5617661820756141E-2</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="29">
         <v>-8.9386491049690764E-2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="B3" s="30">
+      <c r="A3" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="29">
         <v>-2.4202355199732906E-2</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="29">
         <v>7.277922514497015E-2</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="29">
         <v>6.1349400009080846E-3</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="B4" s="30">
+      <c r="A4" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="29">
         <v>-9.4527828992855278E-3</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="29">
         <v>-1.0922625530115693E-2</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="29">
         <v>-1.0230686295118474E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="30">
+      <c r="A5" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="29">
         <v>1.957902819000279E-2</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="29">
         <v>-4.8573189936511607E-2</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="29">
         <v>-2.0327929432213954E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" s="30">
+      <c r="A6" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="29">
         <v>-0.13082254612170008</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="29">
         <v>8.0548284713528595E-3</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="29">
         <v>-0.10101897519046421</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="29" t="s">
-        <v>203</v>
-      </c>
-      <c r="B7" s="30">
+      <c r="A7" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="29">
         <v>-1.3146380955662007E-2</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="29">
         <v>4.9278608154151859E-2</v>
       </c>
-      <c r="D7" s="30">
+      <c r="D7" s="29">
         <v>1.8207196455272578E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="29" t="s">
-        <v>204</v>
-      </c>
-      <c r="B8" s="30">
+      <c r="A8" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="29">
         <v>-1.3400977497078914E-3</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="29">
         <v>-1.3033129323763992E-2</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <v>-3.1569684812242649E-3</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="29" t="s">
-        <v>205</v>
-      </c>
-      <c r="B9" s="30">
+      <c r="A9" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="29">
         <v>8.6045091610129631E-3</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="29">
         <v>-2.3038979195998732E-2</v>
       </c>
-      <c r="D9" s="30">
+      <c r="D9" s="29">
         <v>7.2312211083909173E-3</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="29" t="s">
-        <v>206</v>
-      </c>
-      <c r="B10" s="30">
+      <c r="A10" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="29">
         <v>-2.0373768670736148E-3</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="29">
         <v>-7.1588720167111264E-2</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="29">
         <v>-4.9387447796636286E-2</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="29" t="s">
-        <v>207</v>
-      </c>
-      <c r="B11" s="30">
+      <c r="A11" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="29">
         <v>-7.4506039062984031E-2</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="29">
         <v>-0.10853353024529477</v>
       </c>
-      <c r="D11" s="30">
+      <c r="D11" s="29">
         <v>-9.3137509888338577E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="29" t="s">
-        <v>208</v>
-      </c>
-      <c r="B12" s="30">
+      <c r="A12" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="29">
         <v>1.5926539787773253E-2</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="29">
         <v>-3.6165337853945378E-2</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="29">
         <v>-3.2779353873625294E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="29" t="s">
-        <v>209</v>
-      </c>
-      <c r="B13" s="30">
+      <c r="A13" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" s="29">
         <v>-3.3194663946651382E-2</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="29">
         <v>-4.1867135095641883E-2</v>
       </c>
-      <c r="D13" s="30">
+      <c r="D13" s="29">
         <v>-3.6947896536471125E-2</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="29" t="s">
-        <v>210</v>
-      </c>
-      <c r="B14" s="30">
+      <c r="A14" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="29">
         <v>-5.2234484717663454E-2</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="29">
         <v>-1.9887767507147158E-2</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="29">
         <v>-4.5612608726683712E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="29" t="s">
-        <v>211</v>
-      </c>
-      <c r="B15" s="30">
+      <c r="A15" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" s="29">
         <v>-8.3842121111726176E-2</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="29">
         <v>1.0671354147059109E-2</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="29">
         <v>-7.3834025692786187E-2</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="B16" s="30">
+      <c r="A16" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" s="29">
         <v>-2.0634762341944279E-2</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="29">
         <v>-4.2886013787892807E-3</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="29">
         <v>-8.6808332428619517E-3</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="29" t="s">
-        <v>213</v>
-      </c>
-      <c r="B17" s="30">
+      <c r="A17" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="29">
         <v>1.2220207025338103E-2</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="29">
         <v>-5.6085072130316105E-2</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="29">
         <v>3.1768822601314639E-3</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="29" t="s">
-        <v>214</v>
-      </c>
-      <c r="B18" s="30">
+      <c r="A18" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" s="29">
         <v>-2.3939163436452526E-2</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="29">
         <v>1.5664912442679979E-2</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="29">
         <v>-1.9330226139112172E-2</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="B19" s="30">
+      <c r="A19" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="29">
         <v>-1.1337314760303197E-2</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="29">
         <v>-4.8286935131272468E-2</v>
       </c>
-      <c r="D19" s="30">
+      <c r="D19" s="29">
         <v>-2.1414476539736493E-2</v>
       </c>
     </row>
@@ -49346,10 +50013,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE529FD-4597-F641-B496-01BE3204D79B}">
-  <dimension ref="A1:E125"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="E125" sqref="E125"/>
+    <sheetView topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -51275,6 +51942,17 @@
         <v>40.229999999999997</v>
       </c>
     </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="3">
+        <v>44612</v>
+      </c>
+      <c r="B126">
+        <v>7.42</v>
+      </c>
+      <c r="E126">
+        <v>40.06</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -51282,10 +51960,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5DA751-8DDE-2444-A8CE-DEF963043B5D}">
-  <dimension ref="A1:J383"/>
+  <dimension ref="A1:J389"/>
   <sheetViews>
-    <sheetView topLeftCell="A360" workbookViewId="0">
-      <selection activeCell="E371" sqref="E371"/>
+    <sheetView topLeftCell="A375" workbookViewId="0">
+      <selection activeCell="A385" sqref="A385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -63546,6 +64224,198 @@
         <v>66.569999999999993</v>
       </c>
     </row>
+    <row r="384" spans="1:10">
+      <c r="A384" s="3">
+        <v>44612</v>
+      </c>
+      <c r="B384">
+        <v>61.52</v>
+      </c>
+      <c r="C384">
+        <v>53.17</v>
+      </c>
+      <c r="D384">
+        <v>66.06</v>
+      </c>
+      <c r="E384">
+        <v>61.09</v>
+      </c>
+      <c r="F384">
+        <v>53.14</v>
+      </c>
+      <c r="G384">
+        <v>65.260000000000005</v>
+      </c>
+      <c r="H384">
+        <v>61.81</v>
+      </c>
+      <c r="I384">
+        <v>53.19</v>
+      </c>
+      <c r="J384">
+        <v>66.569999999999993</v>
+      </c>
+    </row>
+    <row r="385" spans="1:10">
+      <c r="A385" s="3">
+        <v>44613</v>
+      </c>
+      <c r="B385">
+        <v>61.7</v>
+      </c>
+      <c r="C385">
+        <v>53.5</v>
+      </c>
+      <c r="D385">
+        <v>66.42</v>
+      </c>
+      <c r="E385">
+        <v>61.09</v>
+      </c>
+      <c r="F385">
+        <v>53.14</v>
+      </c>
+      <c r="G385">
+        <v>65.73</v>
+      </c>
+      <c r="H385">
+        <v>62.1</v>
+      </c>
+      <c r="I385">
+        <v>53.74</v>
+      </c>
+      <c r="J385">
+        <v>66.87</v>
+      </c>
+    </row>
+    <row r="386" spans="1:10">
+      <c r="A386" s="3">
+        <v>44614</v>
+      </c>
+      <c r="B386">
+        <v>62.06</v>
+      </c>
+      <c r="C386">
+        <v>53.67</v>
+      </c>
+      <c r="D386">
+        <v>66.239999999999995</v>
+      </c>
+      <c r="E386">
+        <v>61.54</v>
+      </c>
+      <c r="F386">
+        <v>53.14</v>
+      </c>
+      <c r="G386">
+        <v>65.73</v>
+      </c>
+      <c r="H386">
+        <v>62.39</v>
+      </c>
+      <c r="I386">
+        <v>54.02</v>
+      </c>
+      <c r="J386">
+        <v>66.569999999999993</v>
+      </c>
+    </row>
+    <row r="387" spans="1:10">
+      <c r="A387" s="3">
+        <v>44615</v>
+      </c>
+      <c r="B387">
+        <v>62.23</v>
+      </c>
+      <c r="C387">
+        <v>53.67</v>
+      </c>
+      <c r="D387">
+        <v>66.42</v>
+      </c>
+      <c r="E387">
+        <v>61.99</v>
+      </c>
+      <c r="F387">
+        <v>53.14</v>
+      </c>
+      <c r="G387">
+        <v>66.2</v>
+      </c>
+      <c r="H387">
+        <v>62.39</v>
+      </c>
+      <c r="I387">
+        <v>54.02</v>
+      </c>
+      <c r="J387">
+        <v>66.569999999999993</v>
+      </c>
+    </row>
+    <row r="388" spans="1:10">
+      <c r="A388" s="3">
+        <v>44616</v>
+      </c>
+      <c r="B388">
+        <v>62.23</v>
+      </c>
+      <c r="C388">
+        <v>54.17</v>
+      </c>
+      <c r="D388">
+        <v>66.42</v>
+      </c>
+      <c r="E388">
+        <v>61.99</v>
+      </c>
+      <c r="F388">
+        <v>53.56</v>
+      </c>
+      <c r="G388">
+        <v>66.2</v>
+      </c>
+      <c r="H388">
+        <v>62.39</v>
+      </c>
+      <c r="I388">
+        <v>54.57</v>
+      </c>
+      <c r="J388">
+        <v>66.569999999999993</v>
+      </c>
+    </row>
+    <row r="389" spans="1:10">
+      <c r="A389" s="3">
+        <v>44617</v>
+      </c>
+      <c r="B389">
+        <v>62.41</v>
+      </c>
+      <c r="C389">
+        <v>54.17</v>
+      </c>
+      <c r="D389">
+        <v>66.61</v>
+      </c>
+      <c r="E389">
+        <v>61.99</v>
+      </c>
+      <c r="F389">
+        <v>53.56</v>
+      </c>
+      <c r="G389">
+        <v>66.2</v>
+      </c>
+      <c r="H389">
+        <v>62.68</v>
+      </c>
+      <c r="I389">
+        <v>54.57</v>
+      </c>
+      <c r="J389">
+        <v>66.87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tracker for 27 march
</commit_message>
<xml_diff>
--- a/Manual/input-data.xlsx
+++ b/Manual/input-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vibhav/Documents/Projects/nimf-tracker-git/nimf-tracker/Manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D33C2E-3497-9E46-BF20-06D27D95F01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4AAD444-5B43-3449-9969-1C51C410F89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22400" yWindow="10160" windowWidth="11200" windowHeight="9660" firstSheet="9" activeTab="12" xr2:uid="{D619B3DC-10A9-6C4B-8E47-54B1B3814066}"/>
+    <workbookView xWindow="22400" yWindow="10180" windowWidth="11200" windowHeight="9660" activeTab="2" xr2:uid="{D619B3DC-10A9-6C4B-8E47-54B1B3814066}"/>
   </bookViews>
   <sheets>
     <sheet name="gst-eway" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="146">
   <si>
     <t>e-Way</t>
   </si>
@@ -477,6 +477,18 @@
   <si>
     <t>45-59 Years</t>
   </si>
+  <si>
+    <t>12-14 Years</t>
+  </si>
+  <si>
+    <t>1 </t>
+  </si>
+  <si>
+    <t>3 </t>
+  </si>
+  <si>
+    <t>4 </t>
+  </si>
 </sst>
 </file>
 
@@ -607,9 +619,8 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="16"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF333333"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -656,7 +667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -694,7 +705,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3821,9 +3834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC6F5E2-B870-4348-99F8-4B5FD1019E5B}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5048,10 +5061,10 @@
         <v>2883260</v>
       </c>
       <c r="J35" s="16">
-        <v>26910</v>
+        <v>21572</v>
       </c>
       <c r="K35" s="16">
-        <v>15830</v>
+        <v>13220</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -5076,8 +5089,12 @@
       <c r="G36" s="16"/>
       <c r="H36" s="16"/>
       <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
+      <c r="J36" s="16">
+        <v>22460</v>
+      </c>
+      <c r="K36" s="16">
+        <v>13910</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5086,11 +5103,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F84EB-1F73-1245-BB50-FDD52D41BDBE}">
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5821,6 +5838,17 @@
         <v>8.9700000000000006</v>
       </c>
     </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="3">
+        <v>44631</v>
+      </c>
+      <c r="B67" s="5">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="C67" s="5">
+        <v>9.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5828,10 +5856,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC45300-6A73-FD40-9CA1-0A8697567D0E}">
-  <dimension ref="A1:B132"/>
+  <dimension ref="A1:B134"/>
   <sheetViews>
     <sheetView topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="B128" sqref="B128"/>
+      <selection activeCell="A134" sqref="A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6895,6 +6923,22 @@
         <v>46499510</v>
       </c>
     </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="3">
+        <v>44631</v>
+      </c>
+      <c r="B133" s="16">
+        <v>46059870</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="3">
+        <v>44638</v>
+      </c>
+      <c r="B134" s="34">
+        <v>45439590</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6902,11 +6946,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5353B576-38C4-E445-9E6D-988228532D05}">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
+      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7976,6 +8020,17 @@
       </c>
       <c r="C97">
         <v>7.91</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="4">
+        <v>44631</v>
+      </c>
+      <c r="B98" s="5">
+        <v>8.84</v>
+      </c>
+      <c r="C98" s="5">
+        <v>8.52</v>
       </c>
     </row>
   </sheetData>
@@ -7987,7 +8042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F0D774-4FB9-484A-8B9C-C85D078E33FB}">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
@@ -8012,15 +8067,25 @@
       <c r="B2" s="19">
         <v>2</v>
       </c>
+      <c r="C2" s="19"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19">
+        <v>129</v>
+      </c>
+      <c r="J2" s="19"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:17" ht="18">
       <c r="A3" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B3" s="19">
-        <v>633</v>
+        <v>395</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -8028,11 +8093,13 @@
       <c r="F3" s="20"/>
       <c r="G3" s="19"/>
       <c r="H3" s="20"/>
-      <c r="I3" s="19"/>
+      <c r="I3" s="19">
+        <v>14730</v>
+      </c>
       <c r="J3" s="19"/>
       <c r="K3" s="21"/>
       <c r="L3" s="21"/>
-      <c r="M3" s="20"/>
+      <c r="M3" s="21"/>
       <c r="N3" s="19"/>
       <c r="O3" s="19"/>
       <c r="P3" s="21"/>
@@ -8043,7 +8110,7 @@
         <v>70</v>
       </c>
       <c r="B4" s="19">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="19"/>
@@ -8051,11 +8118,13 @@
       <c r="F4" s="20"/>
       <c r="G4" s="19"/>
       <c r="H4" s="20"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="21"/>
+      <c r="I4" s="19">
+        <v>296</v>
+      </c>
+      <c r="J4" s="19"/>
       <c r="K4" s="21"/>
       <c r="L4" s="21"/>
-      <c r="M4" s="20"/>
+      <c r="M4" s="21"/>
       <c r="N4" s="19"/>
       <c r="O4" s="21"/>
       <c r="P4" s="21"/>
@@ -8066,7 +8135,7 @@
         <v>71</v>
       </c>
       <c r="B5" s="19">
-        <v>1366</v>
+        <v>1362</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
@@ -8074,11 +8143,13 @@
       <c r="F5" s="20"/>
       <c r="G5" s="19"/>
       <c r="H5" s="20"/>
-      <c r="I5" s="19"/>
+      <c r="I5" s="19">
+        <v>6639</v>
+      </c>
       <c r="J5" s="19"/>
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
-      <c r="M5" s="20"/>
+      <c r="M5" s="21"/>
       <c r="N5" s="19"/>
       <c r="O5" s="19"/>
       <c r="P5" s="21"/>
@@ -8089,7 +8160,7 @@
         <v>72</v>
       </c>
       <c r="B6" s="19">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -8097,11 +8168,13 @@
       <c r="F6" s="20"/>
       <c r="G6" s="19"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="19"/>
+      <c r="I6" s="19">
+        <v>12256</v>
+      </c>
       <c r="J6" s="19"/>
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
-      <c r="M6" s="20"/>
+      <c r="M6" s="21"/>
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
       <c r="P6" s="21"/>
@@ -8112,19 +8185,21 @@
         <v>62</v>
       </c>
       <c r="B7" s="19">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
-      <c r="F7" s="20"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="19"/>
       <c r="H7" s="20"/>
-      <c r="I7" s="19"/>
+      <c r="I7" s="19">
+        <v>1165</v>
+      </c>
       <c r="J7" s="19"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
-      <c r="M7" s="20"/>
+      <c r="M7" s="21"/>
       <c r="N7" s="19"/>
       <c r="O7" s="19"/>
       <c r="P7" s="21"/>
@@ -8135,19 +8210,21 @@
         <v>73</v>
       </c>
       <c r="B8" s="19">
-        <v>374</v>
+        <v>147</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="19"/>
       <c r="H8" s="20"/>
-      <c r="I8" s="19"/>
+      <c r="I8" s="19">
+        <v>14034</v>
+      </c>
       <c r="J8" s="19"/>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
-      <c r="M8" s="20"/>
+      <c r="M8" s="21"/>
       <c r="N8" s="19"/>
       <c r="O8" s="19"/>
       <c r="P8" s="21"/>
@@ -8163,14 +8240,16 @@
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19">
+        <v>4</v>
+      </c>
       <c r="J9" s="19"/>
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
-      <c r="M9" s="20"/>
+      <c r="M9" s="21"/>
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>
       <c r="P9" s="21"/>
@@ -8181,19 +8260,21 @@
         <v>75</v>
       </c>
       <c r="B10" s="19">
-        <v>792</v>
+        <v>464</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="19">
+        <v>26150</v>
+      </c>
       <c r="J10" s="19"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
-      <c r="M10" s="19"/>
+      <c r="M10" s="21"/>
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
       <c r="P10" s="21"/>
@@ -8204,19 +8285,21 @@
         <v>76</v>
       </c>
       <c r="B11" s="19">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="19"/>
       <c r="H11" s="20"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="21"/>
+      <c r="I11" s="19">
+        <v>3830</v>
+      </c>
+      <c r="J11" s="19"/>
       <c r="K11" s="21"/>
       <c r="L11" s="21"/>
-      <c r="M11" s="20"/>
+      <c r="M11" s="21"/>
       <c r="N11" s="19"/>
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
@@ -8227,7 +8310,7 @@
         <v>77</v>
       </c>
       <c r="B12" s="19">
-        <v>560</v>
+        <v>276</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
@@ -8235,11 +8318,13 @@
       <c r="F12" s="20"/>
       <c r="G12" s="19"/>
       <c r="H12" s="20"/>
-      <c r="I12" s="19"/>
+      <c r="I12" s="19">
+        <v>10942</v>
+      </c>
       <c r="J12" s="19"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
-      <c r="M12" s="20"/>
+      <c r="M12" s="21"/>
       <c r="N12" s="19"/>
       <c r="O12" s="19"/>
       <c r="P12" s="21"/>
@@ -8250,7 +8335,7 @@
         <v>78</v>
       </c>
       <c r="B13" s="19">
-        <v>813</v>
+        <v>390</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -8258,11 +8343,17 @@
       <c r="F13" s="20"/>
       <c r="G13" s="19"/>
       <c r="H13" s="20"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
+      <c r="I13" s="19">
+        <v>10607</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>145</v>
+      </c>
       <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="20"/>
+      <c r="L13" s="21">
+        <v>4</v>
+      </c>
+      <c r="M13" s="21"/>
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>
       <c r="P13" s="21"/>
@@ -8273,7 +8364,7 @@
         <v>79</v>
       </c>
       <c r="B14" s="19">
-        <v>437</v>
+        <v>191</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -8281,11 +8372,13 @@
       <c r="F14" s="20"/>
       <c r="G14" s="19"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="21"/>
+      <c r="I14" s="19">
+        <v>4132</v>
+      </c>
+      <c r="J14" s="19"/>
       <c r="K14" s="21"/>
       <c r="L14" s="21"/>
-      <c r="M14" s="20"/>
+      <c r="M14" s="21"/>
       <c r="N14" s="19"/>
       <c r="O14" s="21"/>
       <c r="P14" s="21"/>
@@ -8296,19 +8389,21 @@
         <v>80</v>
       </c>
       <c r="B15" s="19">
-        <v>252</v>
+        <v>138</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="19"/>
       <c r="H15" s="20"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="21"/>
+      <c r="I15" s="19">
+        <v>4750</v>
+      </c>
+      <c r="J15" s="19"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
-      <c r="M15" s="20"/>
+      <c r="M15" s="21"/>
       <c r="N15" s="19"/>
       <c r="O15" s="21"/>
       <c r="P15" s="21"/>
@@ -8319,19 +8414,21 @@
         <v>81</v>
       </c>
       <c r="B16" s="19">
-        <v>245</v>
+        <v>78</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="19"/>
       <c r="H16" s="20"/>
-      <c r="I16" s="19"/>
+      <c r="I16" s="19">
+        <v>5315</v>
+      </c>
       <c r="J16" s="19"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
-      <c r="M16" s="20"/>
+      <c r="M16" s="21"/>
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
       <c r="P16" s="21"/>
@@ -8342,7 +8439,7 @@
         <v>82</v>
       </c>
       <c r="B17" s="19">
-        <v>2661</v>
+        <v>1818</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -8350,11 +8447,17 @@
       <c r="F17" s="20"/>
       <c r="G17" s="19"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
+      <c r="I17" s="19">
+        <v>40049</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>143</v>
+      </c>
       <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="20"/>
+      <c r="L17" s="21">
+        <v>1</v>
+      </c>
+      <c r="M17" s="21"/>
       <c r="N17" s="19"/>
       <c r="O17" s="19"/>
       <c r="P17" s="21"/>
@@ -8365,7 +8468,7 @@
         <v>109</v>
       </c>
       <c r="B18" s="19">
-        <v>10350</v>
+        <v>4881</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -8373,11 +8476,19 @@
       <c r="F18" s="20"/>
       <c r="G18" s="19"/>
       <c r="H18" s="20"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="20"/>
+      <c r="I18" s="19">
+        <v>67772</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="K18" s="21">
+        <v>138</v>
+      </c>
+      <c r="L18" s="21">
+        <v>141</v>
+      </c>
+      <c r="M18" s="21"/>
       <c r="N18" s="19"/>
       <c r="O18" s="21"/>
       <c r="P18" s="21"/>
@@ -8388,7 +8499,7 @@
         <v>83</v>
       </c>
       <c r="B19" s="19">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
@@ -8396,11 +8507,13 @@
       <c r="F19" s="20"/>
       <c r="G19" s="19"/>
       <c r="H19" s="20"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="21"/>
+      <c r="I19" s="19">
+        <v>228</v>
+      </c>
+      <c r="J19" s="19"/>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
-      <c r="M19" s="20"/>
+      <c r="M19" s="21"/>
       <c r="N19" s="19"/>
       <c r="O19" s="21"/>
       <c r="P19" s="21"/>
@@ -8411,19 +8524,21 @@
         <v>84</v>
       </c>
       <c r="B20" s="19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
-      <c r="F20" s="20"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="19"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19">
+        <v>52</v>
+      </c>
       <c r="J20" s="19"/>
       <c r="K20" s="21"/>
       <c r="L20" s="21"/>
-      <c r="M20" s="20"/>
+      <c r="M20" s="21"/>
       <c r="N20" s="19"/>
       <c r="O20" s="19"/>
       <c r="P20" s="21"/>
@@ -8434,19 +8549,21 @@
         <v>85</v>
       </c>
       <c r="B21" s="19">
-        <v>678</v>
+        <v>118</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
+      <c r="F21" s="20"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="19">
+        <v>10734</v>
+      </c>
       <c r="J21" s="19"/>
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
-      <c r="M21" s="19"/>
+      <c r="M21" s="21"/>
       <c r="N21" s="19"/>
       <c r="O21" s="19"/>
       <c r="P21" s="21"/>
@@ -8457,19 +8574,21 @@
         <v>86</v>
       </c>
       <c r="B22" s="19">
-        <v>6725</v>
+        <v>893</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="19"/>
       <c r="H22" s="20"/>
-      <c r="I22" s="19"/>
+      <c r="I22" s="19">
+        <v>147779</v>
+      </c>
       <c r="J22" s="19"/>
       <c r="K22" s="21"/>
       <c r="L22" s="21"/>
-      <c r="M22" s="20"/>
+      <c r="M22" s="21"/>
       <c r="N22" s="19"/>
       <c r="O22" s="19"/>
       <c r="P22" s="21"/>
@@ -8480,19 +8599,21 @@
         <v>87</v>
       </c>
       <c r="B23" s="19">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="19"/>
       <c r="H23" s="20"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="21"/>
+      <c r="I23" s="19">
+        <v>2120</v>
+      </c>
+      <c r="J23" s="19"/>
       <c r="K23" s="21"/>
       <c r="L23" s="21"/>
-      <c r="M23" s="20"/>
+      <c r="M23" s="21"/>
       <c r="N23" s="19"/>
       <c r="O23" s="21"/>
       <c r="P23" s="21"/>
@@ -8503,7 +8624,7 @@
         <v>88</v>
       </c>
       <c r="B24" s="19">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
@@ -8511,11 +8632,13 @@
       <c r="F24" s="20"/>
       <c r="G24" s="19"/>
       <c r="H24" s="20"/>
-      <c r="I24" s="19"/>
+      <c r="I24" s="19">
+        <v>1593</v>
+      </c>
       <c r="J24" s="19"/>
       <c r="K24" s="21"/>
       <c r="L24" s="21"/>
-      <c r="M24" s="20"/>
+      <c r="M24" s="21"/>
       <c r="N24" s="19"/>
       <c r="O24" s="19"/>
       <c r="P24" s="21"/>
@@ -8526,7 +8649,7 @@
         <v>89</v>
       </c>
       <c r="B25" s="19">
-        <v>3352</v>
+        <v>1227</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
@@ -8534,11 +8657,17 @@
       <c r="F25" s="20"/>
       <c r="G25" s="19"/>
       <c r="H25" s="20"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
+      <c r="I25" s="19">
+        <v>681</v>
+      </c>
+      <c r="J25" s="21" t="s">
+        <v>143</v>
+      </c>
       <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="20"/>
+      <c r="L25" s="21">
+        <v>1</v>
+      </c>
+      <c r="M25" s="21"/>
       <c r="N25" s="19"/>
       <c r="O25" s="19"/>
       <c r="P25" s="21"/>
@@ -8549,7 +8678,7 @@
         <v>90</v>
       </c>
       <c r="B26" s="19">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
@@ -8557,11 +8686,13 @@
       <c r="F26" s="20"/>
       <c r="G26" s="19"/>
       <c r="H26" s="20"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="21"/>
+      <c r="I26" s="19">
+        <v>758</v>
+      </c>
+      <c r="J26" s="19"/>
       <c r="K26" s="21"/>
       <c r="L26" s="21"/>
-      <c r="M26" s="20"/>
+      <c r="M26" s="21"/>
       <c r="N26" s="19"/>
       <c r="O26" s="21"/>
       <c r="P26" s="21"/>
@@ -8572,19 +8703,25 @@
         <v>91</v>
       </c>
       <c r="B27" s="19">
-        <v>867</v>
+        <v>484</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
       <c r="E27" s="19"/>
-      <c r="F27" s="20"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="19"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19">
+        <v>9118</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>143</v>
+      </c>
       <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="20"/>
+      <c r="L27" s="21">
+        <v>1</v>
+      </c>
+      <c r="M27" s="21"/>
       <c r="N27" s="19"/>
       <c r="O27" s="19"/>
       <c r="P27" s="21"/>
@@ -8595,7 +8732,7 @@
         <v>92</v>
       </c>
       <c r="B28" s="19">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -8603,11 +8740,13 @@
       <c r="F28" s="20"/>
       <c r="G28" s="19"/>
       <c r="H28" s="20"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="21"/>
+      <c r="I28" s="19">
+        <v>1962</v>
+      </c>
+      <c r="J28" s="19"/>
       <c r="K28" s="21"/>
       <c r="L28" s="21"/>
-      <c r="M28" s="20"/>
+      <c r="M28" s="21"/>
       <c r="N28" s="19"/>
       <c r="O28" s="21"/>
       <c r="P28" s="21"/>
@@ -8618,7 +8757,7 @@
         <v>93</v>
       </c>
       <c r="B29" s="19">
-        <v>254</v>
+        <v>113</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
@@ -8626,11 +8765,13 @@
       <c r="F29" s="20"/>
       <c r="G29" s="19"/>
       <c r="H29" s="20"/>
-      <c r="I29" s="19"/>
+      <c r="I29" s="19">
+        <v>17740</v>
+      </c>
       <c r="J29" s="19"/>
       <c r="K29" s="21"/>
       <c r="L29" s="21"/>
-      <c r="M29" s="20"/>
+      <c r="M29" s="21"/>
       <c r="N29" s="19"/>
       <c r="O29" s="19"/>
       <c r="P29" s="21"/>
@@ -8641,7 +8782,7 @@
         <v>94</v>
       </c>
       <c r="B30" s="19">
-        <v>1109</v>
+        <v>271</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -8649,11 +8790,13 @@
       <c r="F30" s="20"/>
       <c r="G30" s="19"/>
       <c r="H30" s="20"/>
-      <c r="I30" s="19"/>
+      <c r="I30" s="19">
+        <v>9551</v>
+      </c>
       <c r="J30" s="19"/>
       <c r="K30" s="21"/>
       <c r="L30" s="21"/>
-      <c r="M30" s="20"/>
+      <c r="M30" s="21"/>
       <c r="N30" s="19"/>
       <c r="O30" s="19"/>
       <c r="P30" s="21"/>
@@ -8664,19 +8807,21 @@
         <v>95</v>
       </c>
       <c r="B31" s="19">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
-      <c r="F31" s="20"/>
+      <c r="F31" s="21"/>
       <c r="G31" s="19"/>
       <c r="H31" s="20"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="21"/>
+      <c r="I31" s="19">
+        <v>451</v>
+      </c>
+      <c r="J31" s="19"/>
       <c r="K31" s="21"/>
       <c r="L31" s="21"/>
-      <c r="M31" s="20"/>
+      <c r="M31" s="21"/>
       <c r="N31" s="19"/>
       <c r="O31" s="21"/>
       <c r="P31" s="21"/>
@@ -8687,7 +8832,7 @@
         <v>96</v>
       </c>
       <c r="B32" s="19">
-        <v>1301</v>
+        <v>418</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -8695,11 +8840,13 @@
       <c r="F32" s="20"/>
       <c r="G32" s="19"/>
       <c r="H32" s="20"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="21"/>
+      <c r="I32" s="19">
+        <v>38025</v>
+      </c>
+      <c r="J32" s="19"/>
       <c r="K32" s="21"/>
       <c r="L32" s="21"/>
-      <c r="M32" s="20"/>
+      <c r="M32" s="21"/>
       <c r="N32" s="19"/>
       <c r="O32" s="21"/>
       <c r="P32" s="21"/>
@@ -8710,7 +8857,7 @@
         <v>97</v>
       </c>
       <c r="B33" s="19">
-        <v>1064</v>
+        <v>536</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -8718,11 +8865,13 @@
       <c r="F33" s="20"/>
       <c r="G33" s="19"/>
       <c r="H33" s="20"/>
-      <c r="I33" s="19"/>
+      <c r="I33" s="19">
+        <v>4111</v>
+      </c>
       <c r="J33" s="19"/>
       <c r="K33" s="21"/>
       <c r="L33" s="21"/>
-      <c r="M33" s="20"/>
+      <c r="M33" s="21"/>
       <c r="N33" s="19"/>
       <c r="O33" s="19"/>
       <c r="P33" s="21"/>
@@ -8733,19 +8882,21 @@
         <v>98</v>
       </c>
       <c r="B34" s="19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
-      <c r="F34" s="20"/>
+      <c r="F34" s="19"/>
       <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19">
+        <v>919</v>
+      </c>
       <c r="J34" s="19"/>
       <c r="K34" s="21"/>
       <c r="L34" s="21"/>
-      <c r="M34" s="20"/>
+      <c r="M34" s="21"/>
       <c r="N34" s="19"/>
       <c r="O34" s="19"/>
       <c r="P34" s="21"/>
@@ -8756,7 +8907,7 @@
         <v>99</v>
       </c>
       <c r="B35" s="19">
-        <v>680</v>
+        <v>519</v>
       </c>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -8764,11 +8915,13 @@
       <c r="F35" s="20"/>
       <c r="G35" s="19"/>
       <c r="H35" s="20"/>
-      <c r="I35" s="19"/>
+      <c r="I35" s="19">
+        <v>7691</v>
+      </c>
       <c r="J35" s="19"/>
       <c r="K35" s="21"/>
       <c r="L35" s="21"/>
-      <c r="M35" s="20"/>
+      <c r="M35" s="21"/>
       <c r="N35" s="19"/>
       <c r="O35" s="19"/>
       <c r="P35" s="21"/>
@@ -8779,19 +8932,25 @@
         <v>100</v>
       </c>
       <c r="B36" s="19">
-        <v>1401</v>
+        <v>490</v>
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="20"/>
       <c r="G36" s="19"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19">
+        <v>23494</v>
+      </c>
+      <c r="J36" s="21" t="s">
+        <v>143</v>
+      </c>
       <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="20"/>
+      <c r="L36" s="21">
+        <v>1</v>
+      </c>
+      <c r="M36" s="21"/>
       <c r="N36" s="19"/>
       <c r="O36" s="19"/>
       <c r="P36" s="21"/>
@@ -8802,7 +8961,7 @@
         <v>101</v>
       </c>
       <c r="B37" s="19">
-        <v>1502</v>
+        <v>729</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
@@ -8810,11 +8969,10 @@
       <c r="F37" s="20"/>
       <c r="G37" s="19"/>
       <c r="H37" s="20"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="20"/>
+      <c r="I37" s="19">
+        <v>21197</v>
+      </c>
+      <c r="J37" s="19"/>
       <c r="N37" s="19"/>
       <c r="O37" s="21"/>
       <c r="P37" s="21"/>
@@ -8844,9 +9002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C1D317E-D501-B04E-B622-A50394A159C7}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
@@ -8875,13 +9031,13 @@
         <v>417036</v>
       </c>
       <c r="C2">
-        <v>328822</v>
+        <v>336234</v>
       </c>
       <c r="D2">
-        <v>322290</v>
+        <v>323602</v>
       </c>
       <c r="E2">
-        <v>9652</v>
+        <v>10252</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -8892,13 +9048,13 @@
         <v>53903393</v>
       </c>
       <c r="C3">
-        <v>43076226</v>
+        <v>44313988</v>
       </c>
       <c r="D3">
-        <v>43097886</v>
+        <v>44983256</v>
       </c>
       <c r="E3">
-        <v>1533568</v>
+        <v>1643791</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -8909,13 +9065,13 @@
         <v>1570458</v>
       </c>
       <c r="C4">
-        <v>890297</v>
+        <v>894651</v>
       </c>
       <c r="D4">
-        <v>730444</v>
+        <v>736426</v>
       </c>
       <c r="E4">
-        <v>24572</v>
+        <v>25406</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -8926,13 +9082,13 @@
         <v>35607039</v>
       </c>
       <c r="C5">
-        <v>23427171</v>
+        <v>23563998</v>
       </c>
       <c r="D5">
-        <v>19923853</v>
+        <v>20110938</v>
       </c>
       <c r="E5">
-        <v>274542</v>
+        <v>291122</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -8943,13 +9099,13 @@
         <v>124799926</v>
       </c>
       <c r="C6">
-        <v>66708539</v>
+        <v>67788000</v>
       </c>
       <c r="D6">
-        <v>54358870</v>
+        <v>55434278</v>
       </c>
       <c r="E6">
-        <v>816212</v>
+        <v>869344</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -8960,13 +9116,13 @@
         <v>1158473</v>
       </c>
       <c r="C7">
-        <v>1125863</v>
+        <v>1130971</v>
       </c>
       <c r="D7">
-        <v>895600</v>
+        <v>902504</v>
       </c>
       <c r="E7">
-        <v>25654</v>
+        <v>27042</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -8977,13 +9133,13 @@
         <v>29436231</v>
       </c>
       <c r="C8">
-        <v>19708013</v>
+        <v>19956586</v>
       </c>
       <c r="D8">
-        <v>17286740</v>
+        <v>17531149</v>
       </c>
       <c r="E8">
-        <v>404538</v>
+        <v>428608</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -8994,13 +9150,13 @@
         <v>18710922</v>
       </c>
       <c r="C9">
-        <v>17334102</v>
+        <v>17668050</v>
       </c>
       <c r="D9">
-        <v>13991320</v>
+        <v>14243116</v>
       </c>
       <c r="E9">
-        <v>444170</v>
+        <v>480184</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -9011,13 +9167,13 @@
         <v>1586250</v>
       </c>
       <c r="C10">
-        <v>1393562</v>
+        <v>1408643</v>
       </c>
       <c r="D10">
-        <v>1229762</v>
+        <v>1235307</v>
       </c>
       <c r="E10">
-        <v>31341</v>
+        <v>32274</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -9028,13 +9184,13 @@
         <v>63872399</v>
       </c>
       <c r="C11">
-        <v>52114051</v>
+        <v>53424876</v>
       </c>
       <c r="D11">
-        <v>49677626</v>
+        <v>50104108</v>
       </c>
       <c r="E11">
-        <v>2174009</v>
+        <v>2310623</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -9045,13 +9201,13 @@
         <v>28204692</v>
       </c>
       <c r="C12">
-        <v>22896374</v>
+        <v>23102569</v>
       </c>
       <c r="D12">
-        <v>18244002</v>
+        <v>18409973</v>
       </c>
       <c r="E12">
-        <v>250475</v>
+        <v>267099</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -9062,13 +9218,13 @@
         <v>7451955</v>
       </c>
       <c r="C13">
-        <v>6325150</v>
+        <v>6457325</v>
       </c>
       <c r="D13">
-        <v>5935064</v>
+        <v>5948858</v>
       </c>
       <c r="E13">
-        <v>185796</v>
+        <v>195909</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -9079,13 +9235,13 @@
         <v>13606320</v>
       </c>
       <c r="C14">
-        <v>10759349</v>
+        <v>10980984</v>
       </c>
       <c r="D14">
-        <v>10622898</v>
+        <v>10760137</v>
       </c>
       <c r="E14">
-        <v>308312</v>
+        <v>325550</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -9096,13 +9252,13 @@
         <v>38593948</v>
       </c>
       <c r="C15">
-        <v>22341014</v>
+        <v>22640284</v>
       </c>
       <c r="D15">
-        <v>14931949</v>
+        <v>15278691</v>
       </c>
       <c r="E15">
-        <v>238844</v>
+        <v>251286</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -9113,13 +9269,13 @@
         <v>67562686</v>
       </c>
       <c r="C16">
-        <v>52197172</v>
+        <v>52794014</v>
       </c>
       <c r="D16">
-        <v>48520112</v>
+        <v>49261230</v>
       </c>
       <c r="E16">
-        <v>1266268</v>
+        <v>1342687</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -9130,13 +9286,13 @@
         <v>35699443</v>
       </c>
       <c r="C17">
-        <v>28120884</v>
+        <v>28180415</v>
       </c>
       <c r="D17">
-        <v>23873182</v>
+        <v>24040347</v>
       </c>
       <c r="E17">
-        <v>958843</v>
+        <v>1100537</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -9147,13 +9303,13 @@
         <v>299000</v>
       </c>
       <c r="C18">
-        <v>227448</v>
+        <v>233611</v>
       </c>
       <c r="D18">
-        <v>188592</v>
+        <v>189377</v>
       </c>
       <c r="E18">
-        <v>31783</v>
+        <v>33347</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -9164,13 +9320,13 @@
         <v>289023</v>
       </c>
       <c r="C19">
-        <v>59528</v>
+        <v>61328</v>
       </c>
       <c r="D19">
-        <v>57121</v>
+        <v>57265</v>
       </c>
       <c r="E19">
-        <v>2520</v>
+        <v>2661</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -9181,13 +9337,13 @@
         <v>85358965</v>
       </c>
       <c r="C20">
-        <v>58009463</v>
+        <v>58955579</v>
       </c>
       <c r="D20">
-        <v>55370484</v>
+        <v>55619464</v>
       </c>
       <c r="E20">
-        <v>912172</v>
+        <v>936893</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -9198,13 +9354,13 @@
         <v>123144223</v>
       </c>
       <c r="C21">
-        <v>87540076</v>
+        <v>88736655</v>
       </c>
       <c r="D21">
-        <v>68471663</v>
+        <v>69820601</v>
       </c>
       <c r="E21">
-        <v>1624397</v>
+        <v>1762346</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -9215,13 +9371,13 @@
         <v>3091545</v>
       </c>
       <c r="C22">
-        <v>1522398</v>
+        <v>1534693</v>
       </c>
       <c r="D22">
-        <v>1165377</v>
+        <v>1178436</v>
       </c>
       <c r="E22">
-        <v>63114</v>
+        <v>65249</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -9232,13 +9388,13 @@
         <v>3366710</v>
       </c>
       <c r="C23">
-        <v>1366620</v>
+        <v>1373735</v>
       </c>
       <c r="D23">
-        <v>982742</v>
+        <v>996334</v>
       </c>
       <c r="E23">
-        <v>28729</v>
+        <v>30120</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -9249,13 +9405,13 @@
         <v>1239244</v>
       </c>
       <c r="C24">
-        <v>825466</v>
+        <v>837752</v>
       </c>
       <c r="D24">
-        <v>654568</v>
+        <v>664197</v>
       </c>
       <c r="E24">
-        <v>24987</v>
+        <v>25896</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -9266,13 +9422,13 @@
         <v>2249695</v>
       </c>
       <c r="C25">
-        <v>876338</v>
+        <v>879408</v>
       </c>
       <c r="D25">
-        <v>660901</v>
+        <v>668065</v>
       </c>
       <c r="E25">
-        <v>22992</v>
+        <v>23902</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -9283,13 +9439,13 @@
         <v>46356334</v>
       </c>
       <c r="C26">
-        <v>32913117</v>
+        <v>33602878</v>
       </c>
       <c r="D26">
-        <v>28203808</v>
+        <v>28770030</v>
       </c>
       <c r="E26">
-        <v>839108</v>
+        <v>897990</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -9300,13 +9456,13 @@
         <v>1413542</v>
       </c>
       <c r="C27">
-        <v>933266</v>
+        <v>945759</v>
       </c>
       <c r="D27">
-        <v>659472</v>
+        <v>672193</v>
       </c>
       <c r="E27">
-        <v>12932</v>
+        <v>13860</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -9317,13 +9473,13 @@
         <v>30141373</v>
       </c>
       <c r="C28">
-        <v>22776840</v>
+        <v>23092716</v>
       </c>
       <c r="D28">
-        <v>16748941</v>
+        <v>17167562</v>
       </c>
       <c r="E28">
-        <v>414819</v>
+        <v>433684</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -9334,13 +9490,13 @@
         <v>81032689</v>
       </c>
       <c r="C29">
-        <v>53963482</v>
+        <v>55295928</v>
       </c>
       <c r="D29">
-        <v>44643003</v>
+        <v>45366745</v>
       </c>
       <c r="E29">
-        <v>1371939</v>
+        <v>1446376</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -9351,13 +9507,13 @@
         <v>690251</v>
       </c>
       <c r="C30">
-        <v>563690</v>
+        <v>569147</v>
       </c>
       <c r="D30">
-        <v>518135</v>
+        <v>520337</v>
       </c>
       <c r="E30">
-        <v>30310</v>
+        <v>31329</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -9368,13 +9524,13 @@
         <v>77841267</v>
       </c>
       <c r="C31">
-        <v>56030623</v>
+        <v>57282606</v>
       </c>
       <c r="D31">
-        <v>43601670</v>
+        <v>44746575</v>
       </c>
       <c r="E31">
-        <v>617393</v>
+        <v>671350</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -9385,13 +9541,13 @@
         <v>38510982</v>
       </c>
       <c r="C32">
-        <v>30938891</v>
+        <v>31643734</v>
       </c>
       <c r="D32">
-        <v>27910958</v>
+        <v>28663700</v>
       </c>
       <c r="E32">
-        <v>502417</v>
+        <v>537477</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -9402,13 +9558,13 @@
         <v>4169794</v>
       </c>
       <c r="C33">
-        <v>2767111</v>
+        <v>2813343</v>
       </c>
       <c r="D33">
-        <v>2288961</v>
+        <v>2298977</v>
       </c>
       <c r="E33">
-        <v>67401</v>
+        <v>70731</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -9419,13 +9575,13 @@
         <v>237882725</v>
       </c>
       <c r="C34">
-        <v>165327049</v>
+        <v>166021617</v>
       </c>
       <c r="D34">
-        <v>126658493</v>
+        <v>129872265</v>
       </c>
       <c r="E34">
-        <v>2334165</v>
+        <v>2391785</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -9436,13 +9592,13 @@
         <v>11250858</v>
       </c>
       <c r="C35">
-        <v>8588431</v>
+        <v>8699242</v>
       </c>
       <c r="D35">
-        <v>7984532</v>
+        <v>8033409</v>
       </c>
       <c r="E35">
-        <v>409063</v>
+        <v>421704</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -9453,13 +9609,13 @@
         <v>99609303</v>
       </c>
       <c r="C36">
-        <v>70145561</v>
+        <v>71282964</v>
       </c>
       <c r="D36">
-        <v>60411268</v>
+        <v>61185978</v>
       </c>
       <c r="E36">
-        <v>1728741</v>
+        <v>1852877</v>
       </c>
     </row>
   </sheetData>
@@ -9469,10 +9625,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8984DF-48CB-5447-B9FA-A4B1DAFD9CF3}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9499,78 +9655,88 @@
       <c r="A2" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="B2" s="33">
-        <v>10402622</v>
-      </c>
-      <c r="C2" s="33">
-        <v>9984407</v>
-      </c>
-      <c r="D2" s="33">
-        <v>4310000</v>
+      <c r="B2" s="35">
+        <v>10403472</v>
+      </c>
+      <c r="C2" s="35">
+        <v>9996261</v>
+      </c>
+      <c r="D2" s="35">
+        <v>4421872</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20">
       <c r="A3" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="33">
-        <v>18411428</v>
-      </c>
-      <c r="C3" s="33">
-        <v>17476822</v>
-      </c>
-      <c r="D3" s="33">
-        <v>6548262</v>
+      <c r="B3" s="35">
+        <v>18412797</v>
+      </c>
+      <c r="C3" s="35">
+        <v>17501086</v>
+      </c>
+      <c r="D3" s="35">
+        <v>6793476</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20">
       <c r="A4" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B4" s="33">
-        <v>55871085</v>
-      </c>
-      <c r="C4" s="33">
-        <v>33770605</v>
-      </c>
-      <c r="D4" s="18"/>
+        <v>142</v>
+      </c>
+      <c r="B4" s="35">
+        <v>12201065</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" ht="20">
       <c r="A5" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="33">
-        <v>553311626</v>
-      </c>
-      <c r="C5" s="33">
-        <v>455201014</v>
+        <v>116</v>
+      </c>
+      <c r="B5" s="35">
+        <v>56814422</v>
+      </c>
+      <c r="C5" s="35">
+        <v>37174113</v>
       </c>
       <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4" ht="20">
       <c r="A6" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B6" s="33">
-        <v>202529223</v>
-      </c>
-      <c r="C6" s="33">
-        <v>182729190</v>
+        <v>117</v>
+      </c>
+      <c r="B6" s="35">
+        <v>554278022</v>
+      </c>
+      <c r="C6" s="35">
+        <v>463457530</v>
       </c>
       <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:4" ht="20">
       <c r="A7" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="35">
+        <v>202690969</v>
+      </c>
+      <c r="C7" s="35">
+        <v>184748950</v>
+      </c>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" spans="1:4" ht="20">
+      <c r="A8" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="B7" s="33">
-        <v>126589403</v>
-      </c>
-      <c r="C7" s="33">
-        <v>113807410</v>
-      </c>
-      <c r="D7" s="33">
-        <v>10380450</v>
+      <c r="B8" s="35">
+        <v>126697598</v>
+      </c>
+      <c r="C8" s="35">
+        <v>115077930</v>
+      </c>
+      <c r="D8" s="35">
+        <v>11340467</v>
       </c>
     </row>
   </sheetData>
@@ -9580,10 +9746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DCA94CA-D9DE-B548-8735-C3641B00F463}">
-  <dimension ref="A1:S341"/>
+  <dimension ref="A1:S352"/>
   <sheetViews>
-    <sheetView topLeftCell="A328" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B336" sqref="B336:S341"/>
+    <sheetView topLeftCell="A339" zoomScale="115" workbookViewId="0">
+      <selection activeCell="B347" sqref="B347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -29707,6 +29873,655 @@
         <v>52000</v>
       </c>
     </row>
+    <row r="342" spans="1:19">
+      <c r="A342" s="3">
+        <v>44634</v>
+      </c>
+      <c r="B342" s="16">
+        <v>22000</v>
+      </c>
+      <c r="C342" s="16">
+        <v>22000</v>
+      </c>
+      <c r="D342" s="16">
+        <v>12500</v>
+      </c>
+      <c r="E342" s="16">
+        <v>35000</v>
+      </c>
+      <c r="F342" s="16">
+        <v>28500</v>
+      </c>
+      <c r="G342" s="16">
+        <v>32000</v>
+      </c>
+      <c r="H342" s="16">
+        <v>18500</v>
+      </c>
+      <c r="I342" s="16">
+        <v>20500</v>
+      </c>
+      <c r="J342" s="16">
+        <v>31500</v>
+      </c>
+      <c r="K342" s="16">
+        <v>31500</v>
+      </c>
+      <c r="L342" s="16">
+        <v>50000</v>
+      </c>
+      <c r="M342" s="16">
+        <v>82000</v>
+      </c>
+      <c r="N342" s="16">
+        <v>63000</v>
+      </c>
+      <c r="O342" s="16">
+        <v>84500</v>
+      </c>
+      <c r="P342" s="16">
+        <v>88000</v>
+      </c>
+      <c r="Q342" s="16">
+        <v>89000</v>
+      </c>
+      <c r="R342" s="16">
+        <v>64000</v>
+      </c>
+      <c r="S342" s="16">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="343" spans="1:19">
+      <c r="A343" s="3">
+        <v>44635</v>
+      </c>
+      <c r="B343" s="16">
+        <v>22000</v>
+      </c>
+      <c r="C343" s="16">
+        <v>22000</v>
+      </c>
+      <c r="D343" s="16">
+        <v>12500</v>
+      </c>
+      <c r="E343" s="16">
+        <v>35000</v>
+      </c>
+      <c r="F343" s="16">
+        <v>28500</v>
+      </c>
+      <c r="G343" s="16">
+        <v>32000</v>
+      </c>
+      <c r="H343" s="16">
+        <v>18500</v>
+      </c>
+      <c r="I343" s="16">
+        <v>20500</v>
+      </c>
+      <c r="J343" s="16">
+        <v>31500</v>
+      </c>
+      <c r="K343" s="16">
+        <v>31500</v>
+      </c>
+      <c r="L343" s="16">
+        <v>50000</v>
+      </c>
+      <c r="M343" s="16">
+        <v>82000</v>
+      </c>
+      <c r="N343" s="16">
+        <v>63000</v>
+      </c>
+      <c r="O343" s="16">
+        <v>84500</v>
+      </c>
+      <c r="P343" s="16">
+        <v>88000</v>
+      </c>
+      <c r="Q343" s="16">
+        <v>89000</v>
+      </c>
+      <c r="R343" s="16">
+        <v>64000</v>
+      </c>
+      <c r="S343" s="16">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="344" spans="1:19">
+      <c r="A344" s="3">
+        <v>44636</v>
+      </c>
+      <c r="B344" s="16">
+        <v>22000</v>
+      </c>
+      <c r="C344" s="16">
+        <v>22000</v>
+      </c>
+      <c r="D344" s="16">
+        <v>12500</v>
+      </c>
+      <c r="E344" s="16">
+        <v>35000</v>
+      </c>
+      <c r="F344" s="16">
+        <v>28500</v>
+      </c>
+      <c r="G344" s="16">
+        <v>32000</v>
+      </c>
+      <c r="H344" s="16">
+        <v>18500</v>
+      </c>
+      <c r="I344" s="16">
+        <v>20500</v>
+      </c>
+      <c r="J344" s="16">
+        <v>31500</v>
+      </c>
+      <c r="K344" s="16">
+        <v>31500</v>
+      </c>
+      <c r="L344" s="16">
+        <v>50500</v>
+      </c>
+      <c r="M344" s="16">
+        <v>82000</v>
+      </c>
+      <c r="N344" s="16">
+        <v>63000</v>
+      </c>
+      <c r="O344" s="16">
+        <v>84500</v>
+      </c>
+      <c r="P344" s="16">
+        <v>88000</v>
+      </c>
+      <c r="Q344" s="16">
+        <v>89000</v>
+      </c>
+      <c r="R344" s="16">
+        <v>64000</v>
+      </c>
+      <c r="S344" s="16">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="345" spans="1:19">
+      <c r="A345" s="3">
+        <v>44637</v>
+      </c>
+      <c r="B345" s="16">
+        <v>22000</v>
+      </c>
+      <c r="C345" s="16">
+        <v>22000</v>
+      </c>
+      <c r="D345" s="16">
+        <v>12500</v>
+      </c>
+      <c r="E345" s="16">
+        <v>35000</v>
+      </c>
+      <c r="F345" s="16">
+        <v>28500</v>
+      </c>
+      <c r="G345" s="16">
+        <v>32000</v>
+      </c>
+      <c r="H345" s="16">
+        <v>18500</v>
+      </c>
+      <c r="I345" s="16">
+        <v>20500</v>
+      </c>
+      <c r="J345" s="16">
+        <v>31500</v>
+      </c>
+      <c r="K345" s="16">
+        <v>31500</v>
+      </c>
+      <c r="L345" s="16">
+        <v>50500</v>
+      </c>
+      <c r="M345" s="16">
+        <v>82000</v>
+      </c>
+      <c r="N345" s="16">
+        <v>63000</v>
+      </c>
+      <c r="O345" s="16">
+        <v>84500</v>
+      </c>
+      <c r="P345" s="16">
+        <v>88000</v>
+      </c>
+      <c r="Q345" s="16">
+        <v>89000</v>
+      </c>
+      <c r="R345" s="16">
+        <v>64000</v>
+      </c>
+      <c r="S345" s="16">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="346" spans="1:19">
+      <c r="A346" s="3">
+        <v>44639</v>
+      </c>
+      <c r="B346" s="16">
+        <v>22000</v>
+      </c>
+      <c r="C346" s="16">
+        <v>22000</v>
+      </c>
+      <c r="D346" s="16">
+        <v>12500</v>
+      </c>
+      <c r="E346" s="16">
+        <v>35000</v>
+      </c>
+      <c r="F346" s="16">
+        <v>28500</v>
+      </c>
+      <c r="G346" s="16">
+        <v>32000</v>
+      </c>
+      <c r="H346" s="16">
+        <v>18500</v>
+      </c>
+      <c r="I346" s="16">
+        <v>20500</v>
+      </c>
+      <c r="J346" s="16">
+        <v>31500</v>
+      </c>
+      <c r="K346" s="16">
+        <v>31500</v>
+      </c>
+      <c r="L346" s="16">
+        <v>50500</v>
+      </c>
+      <c r="M346" s="16">
+        <v>82000</v>
+      </c>
+      <c r="N346" s="16">
+        <v>63000</v>
+      </c>
+      <c r="O346" s="16">
+        <v>84500</v>
+      </c>
+      <c r="P346" s="16">
+        <v>88000</v>
+      </c>
+      <c r="Q346" s="16">
+        <v>89000</v>
+      </c>
+      <c r="R346" s="16">
+        <v>64000</v>
+      </c>
+      <c r="S346" s="16">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="347" spans="1:19">
+      <c r="A347" s="3">
+        <v>44641</v>
+      </c>
+      <c r="B347" s="16">
+        <v>22000</v>
+      </c>
+      <c r="C347" s="16">
+        <v>22000</v>
+      </c>
+      <c r="D347" s="16">
+        <v>12500</v>
+      </c>
+      <c r="E347" s="16">
+        <v>35000</v>
+      </c>
+      <c r="F347" s="16">
+        <v>28500</v>
+      </c>
+      <c r="G347" s="16">
+        <v>32000</v>
+      </c>
+      <c r="H347" s="16">
+        <v>18500</v>
+      </c>
+      <c r="I347" s="16">
+        <v>20500</v>
+      </c>
+      <c r="J347" s="16">
+        <v>31500</v>
+      </c>
+      <c r="K347" s="16">
+        <v>31500</v>
+      </c>
+      <c r="L347" s="16">
+        <v>50500</v>
+      </c>
+      <c r="M347" s="16">
+        <v>82000</v>
+      </c>
+      <c r="N347" s="16">
+        <v>63000</v>
+      </c>
+      <c r="O347" s="16">
+        <v>84500</v>
+      </c>
+      <c r="P347" s="16">
+        <v>88000</v>
+      </c>
+      <c r="Q347" s="16">
+        <v>89000</v>
+      </c>
+      <c r="R347" s="16">
+        <v>64000</v>
+      </c>
+      <c r="S347" s="16">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="348" spans="1:19">
+      <c r="A348" s="3">
+        <v>44642</v>
+      </c>
+      <c r="B348" s="16">
+        <v>22000</v>
+      </c>
+      <c r="C348" s="16">
+        <v>22000</v>
+      </c>
+      <c r="D348" s="16">
+        <v>12500</v>
+      </c>
+      <c r="E348" s="16">
+        <v>35000</v>
+      </c>
+      <c r="F348" s="16">
+        <v>28500</v>
+      </c>
+      <c r="G348" s="16">
+        <v>32000</v>
+      </c>
+      <c r="H348" s="16">
+        <v>18500</v>
+      </c>
+      <c r="I348" s="16">
+        <v>20500</v>
+      </c>
+      <c r="J348" s="16">
+        <v>31500</v>
+      </c>
+      <c r="K348" s="16">
+        <v>31500</v>
+      </c>
+      <c r="L348" s="16">
+        <v>50500</v>
+      </c>
+      <c r="M348" s="16">
+        <v>82000</v>
+      </c>
+      <c r="N348" s="16">
+        <v>63000</v>
+      </c>
+      <c r="O348" s="16">
+        <v>84500</v>
+      </c>
+      <c r="P348" s="16">
+        <v>88000</v>
+      </c>
+      <c r="Q348" s="16">
+        <v>89000</v>
+      </c>
+      <c r="R348" s="16">
+        <v>64000</v>
+      </c>
+      <c r="S348" s="16">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="349" spans="1:19">
+      <c r="A349" s="3">
+        <v>44643</v>
+      </c>
+      <c r="B349" s="16">
+        <v>22000</v>
+      </c>
+      <c r="C349" s="16">
+        <v>22000</v>
+      </c>
+      <c r="D349" s="16">
+        <v>12500</v>
+      </c>
+      <c r="E349" s="16">
+        <v>35000</v>
+      </c>
+      <c r="F349" s="16">
+        <v>28500</v>
+      </c>
+      <c r="G349" s="16">
+        <v>32000</v>
+      </c>
+      <c r="H349" s="16">
+        <v>18500</v>
+      </c>
+      <c r="I349" s="16">
+        <v>20500</v>
+      </c>
+      <c r="J349" s="16">
+        <v>31500</v>
+      </c>
+      <c r="K349" s="16">
+        <v>31500</v>
+      </c>
+      <c r="L349" s="16">
+        <v>50500</v>
+      </c>
+      <c r="M349" s="16">
+        <v>82000</v>
+      </c>
+      <c r="N349" s="16">
+        <v>63000</v>
+      </c>
+      <c r="O349" s="16">
+        <v>84500</v>
+      </c>
+      <c r="P349" s="16">
+        <v>88000</v>
+      </c>
+      <c r="Q349" s="16">
+        <v>89000</v>
+      </c>
+      <c r="R349" s="16">
+        <v>64000</v>
+      </c>
+      <c r="S349" s="16">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="350" spans="1:19">
+      <c r="A350" s="3">
+        <v>44644</v>
+      </c>
+      <c r="B350" s="16">
+        <v>22000</v>
+      </c>
+      <c r="C350" s="16">
+        <v>22000</v>
+      </c>
+      <c r="D350" s="16">
+        <v>12500</v>
+      </c>
+      <c r="E350" s="16">
+        <v>35000</v>
+      </c>
+      <c r="F350" s="16">
+        <v>28500</v>
+      </c>
+      <c r="G350" s="16">
+        <v>32000</v>
+      </c>
+      <c r="H350" s="16">
+        <v>18500</v>
+      </c>
+      <c r="I350" s="16">
+        <v>20500</v>
+      </c>
+      <c r="J350" s="16">
+        <v>31500</v>
+      </c>
+      <c r="K350" s="16">
+        <v>31500</v>
+      </c>
+      <c r="L350" s="16">
+        <v>50500</v>
+      </c>
+      <c r="M350" s="16">
+        <v>82000</v>
+      </c>
+      <c r="N350" s="16">
+        <v>63000</v>
+      </c>
+      <c r="O350" s="16">
+        <v>84500</v>
+      </c>
+      <c r="P350" s="16">
+        <v>88000</v>
+      </c>
+      <c r="Q350" s="16">
+        <v>89000</v>
+      </c>
+      <c r="R350" s="16">
+        <v>64000</v>
+      </c>
+      <c r="S350" s="16">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="351" spans="1:19">
+      <c r="A351" s="3">
+        <v>44645</v>
+      </c>
+      <c r="B351" s="16">
+        <v>22000</v>
+      </c>
+      <c r="C351" s="16">
+        <v>22000</v>
+      </c>
+      <c r="D351" s="16">
+        <v>12500</v>
+      </c>
+      <c r="E351" s="16">
+        <v>35000</v>
+      </c>
+      <c r="F351" s="16">
+        <v>28500</v>
+      </c>
+      <c r="G351" s="16">
+        <v>32000</v>
+      </c>
+      <c r="H351" s="16">
+        <v>18500</v>
+      </c>
+      <c r="I351" s="16">
+        <v>20500</v>
+      </c>
+      <c r="J351" s="16">
+        <v>31500</v>
+      </c>
+      <c r="K351" s="16">
+        <v>31500</v>
+      </c>
+      <c r="L351" s="16">
+        <v>50500</v>
+      </c>
+      <c r="M351" s="16">
+        <v>82000</v>
+      </c>
+      <c r="N351" s="16">
+        <v>63000</v>
+      </c>
+      <c r="O351" s="16">
+        <v>84500</v>
+      </c>
+      <c r="P351" s="16">
+        <v>88000</v>
+      </c>
+      <c r="Q351" s="16">
+        <v>89000</v>
+      </c>
+      <c r="R351" s="16">
+        <v>64000</v>
+      </c>
+      <c r="S351" s="16">
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="352" spans="1:19">
+      <c r="A352" s="3">
+        <v>44646</v>
+      </c>
+      <c r="B352" s="16">
+        <v>22000</v>
+      </c>
+      <c r="C352" s="16">
+        <v>22000</v>
+      </c>
+      <c r="D352" s="16">
+        <v>12500</v>
+      </c>
+      <c r="E352" s="16">
+        <v>35000</v>
+      </c>
+      <c r="F352" s="16">
+        <v>28500</v>
+      </c>
+      <c r="G352" s="16">
+        <v>32000</v>
+      </c>
+      <c r="H352" s="16">
+        <v>18500</v>
+      </c>
+      <c r="I352" s="16">
+        <v>20500</v>
+      </c>
+      <c r="J352" s="16">
+        <v>31500</v>
+      </c>
+      <c r="K352" s="16">
+        <v>31500</v>
+      </c>
+      <c r="L352" s="16">
+        <v>50500</v>
+      </c>
+      <c r="M352" s="16">
+        <v>82000</v>
+      </c>
+      <c r="N352" s="16">
+        <v>63000</v>
+      </c>
+      <c r="O352" s="16">
+        <v>84500</v>
+      </c>
+      <c r="P352" s="16">
+        <v>88000</v>
+      </c>
+      <c r="Q352" s="16">
+        <v>89000</v>
+      </c>
+      <c r="R352" s="16">
+        <v>64000</v>
+      </c>
+      <c r="S352" s="16">
+        <v>52000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29714,10 +30529,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5A5412-72F4-CA4E-9682-44F6B6C554A4}">
-  <dimension ref="A1:B1169"/>
+  <dimension ref="A1:B1182"/>
   <sheetViews>
-    <sheetView topLeftCell="A1155" workbookViewId="0">
-      <selection activeCell="A1167" sqref="A1167"/>
+    <sheetView tabSelected="1" topLeftCell="A1167" workbookViewId="0">
+      <selection activeCell="A1182" sqref="A1182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -39059,10 +39874,124 @@
       </c>
     </row>
     <row r="1168" spans="1:2">
-      <c r="A1168" s="4"/>
-    </row>
-    <row r="1169" spans="1:1">
-      <c r="A1169" s="4"/>
+      <c r="A1168" s="4">
+        <v>44632</v>
+      </c>
+      <c r="B1168">
+        <v>4151</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:2">
+      <c r="A1169" s="4">
+        <v>44633</v>
+      </c>
+      <c r="B1169">
+        <v>4053</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:2">
+      <c r="A1170" s="4">
+        <v>44634</v>
+      </c>
+      <c r="B1170">
+        <v>4220</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:2">
+      <c r="A1171" s="4">
+        <v>44635</v>
+      </c>
+      <c r="B1171">
+        <v>4299</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:2">
+      <c r="A1172" s="4">
+        <v>44636</v>
+      </c>
+      <c r="B1172">
+        <v>4353</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:2">
+      <c r="A1173" s="4">
+        <v>44637</v>
+      </c>
+      <c r="B1173">
+        <v>4358</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:2">
+      <c r="A1174" s="4">
+        <v>44638</v>
+      </c>
+      <c r="B1174">
+        <v>4046</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:2">
+      <c r="A1175" s="4">
+        <v>44639</v>
+      </c>
+      <c r="B1175">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:2">
+      <c r="A1176" s="4">
+        <v>44640</v>
+      </c>
+      <c r="B1176">
+        <v>4152</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:2">
+      <c r="A1177" s="4">
+        <v>44641</v>
+      </c>
+      <c r="B1177">
+        <v>4320</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:2">
+      <c r="A1178" s="4">
+        <v>44642</v>
+      </c>
+      <c r="B1178">
+        <v>4338</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:2">
+      <c r="A1179" s="4">
+        <v>44643</v>
+      </c>
+      <c r="B1179">
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:2">
+      <c r="A1180" s="4">
+        <v>44644</v>
+      </c>
+      <c r="B1180">
+        <v>4329</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:2">
+      <c r="A1181" s="4">
+        <v>44645</v>
+      </c>
+      <c r="B1181">
+        <v>4311</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:2">
+      <c r="A1182" s="4">
+        <v>44646</v>
+      </c>
+      <c r="B1182">
+        <v>4270</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -39071,10 +40000,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D44E43D3-B2B8-4440-9DFA-30FE18FECCE6}">
-  <dimension ref="A1:B650"/>
+  <dimension ref="A1:B664"/>
   <sheetViews>
-    <sheetView topLeftCell="A640" workbookViewId="0">
-      <selection activeCell="A650" sqref="A650"/>
+    <sheetView topLeftCell="A653" workbookViewId="0">
+      <selection activeCell="A654" sqref="A654:A664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -44279,6 +45208,118 @@
         <v>32377.05</v>
       </c>
     </row>
+    <row r="651" spans="1:2">
+      <c r="A651" s="4">
+        <v>44632</v>
+      </c>
+      <c r="B651" s="33">
+        <v>29318.33</v>
+      </c>
+    </row>
+    <row r="652" spans="1:2">
+      <c r="A652" s="4">
+        <v>44633</v>
+      </c>
+      <c r="B652" s="33">
+        <v>23152.81</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2">
+      <c r="A653" s="4">
+        <v>44634</v>
+      </c>
+      <c r="B653" s="33">
+        <v>33957.67</v>
+      </c>
+    </row>
+    <row r="654" spans="1:2">
+      <c r="A654" s="4">
+        <v>44635</v>
+      </c>
+      <c r="B654" s="33">
+        <v>33340.639999999999</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2">
+      <c r="A655" s="4">
+        <v>44636</v>
+      </c>
+      <c r="B655" s="33">
+        <v>33221.879999999997</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2">
+      <c r="A656" s="4">
+        <v>44637</v>
+      </c>
+      <c r="B656" s="33">
+        <v>31166.73</v>
+      </c>
+    </row>
+    <row r="657" spans="1:2">
+      <c r="A657" s="4">
+        <v>44638</v>
+      </c>
+      <c r="B657" s="33">
+        <v>18869.04</v>
+      </c>
+    </row>
+    <row r="658" spans="1:2">
+      <c r="A658" s="4">
+        <v>44639</v>
+      </c>
+      <c r="B658" s="17">
+        <v>25247.27</v>
+      </c>
+    </row>
+    <row r="659" spans="1:2">
+      <c r="A659" s="4">
+        <v>44640</v>
+      </c>
+      <c r="B659" s="17">
+        <v>21237.31</v>
+      </c>
+    </row>
+    <row r="660" spans="1:2">
+      <c r="A660" s="4">
+        <v>44641</v>
+      </c>
+      <c r="B660" s="17">
+        <v>31841.8</v>
+      </c>
+    </row>
+    <row r="661" spans="1:2">
+      <c r="A661" s="4">
+        <v>44642</v>
+      </c>
+      <c r="B661" s="17">
+        <v>29566.9</v>
+      </c>
+    </row>
+    <row r="662" spans="1:2">
+      <c r="A662" s="4">
+        <v>44643</v>
+      </c>
+      <c r="B662" s="17">
+        <v>29859.79</v>
+      </c>
+    </row>
+    <row r="663" spans="1:2">
+      <c r="A663" s="4">
+        <v>44644</v>
+      </c>
+      <c r="B663" s="17">
+        <v>29588.27</v>
+      </c>
+    </row>
+    <row r="664" spans="1:2">
+      <c r="A664" s="4">
+        <v>44645</v>
+      </c>
+      <c r="B664" s="17">
+        <v>29741.97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44286,10 +45327,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D064278-E4AD-8149-B400-6EAC50E0DC3D}">
-  <dimension ref="A1:B574"/>
+  <dimension ref="A1:B588"/>
   <sheetViews>
-    <sheetView topLeftCell="A563" zoomScale="132" workbookViewId="0">
-      <selection activeCell="A574" sqref="A574"/>
+    <sheetView topLeftCell="A577" zoomScale="132" workbookViewId="0">
+      <selection activeCell="A580" sqref="A580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -48884,6 +49925,118 @@
       </c>
       <c r="B574">
         <v>7.37</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2">
+      <c r="A575" s="3">
+        <v>44633</v>
+      </c>
+      <c r="B575">
+        <v>7.38</v>
+      </c>
+    </row>
+    <row r="576" spans="1:2">
+      <c r="A576" s="3">
+        <v>44634</v>
+      </c>
+      <c r="B576">
+        <v>7.24</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2">
+      <c r="A577" s="3">
+        <v>44635</v>
+      </c>
+      <c r="B577">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="578" spans="1:2">
+      <c r="A578" s="3">
+        <v>44636</v>
+      </c>
+      <c r="B578">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2">
+      <c r="A579" s="3">
+        <v>44637</v>
+      </c>
+      <c r="B579">
+        <v>7.23</v>
+      </c>
+    </row>
+    <row r="580" spans="1:2">
+      <c r="A580" s="3">
+        <v>44638</v>
+      </c>
+      <c r="B580">
+        <v>7.38</v>
+      </c>
+    </row>
+    <row r="581" spans="1:2">
+      <c r="A581" s="3">
+        <v>44639</v>
+      </c>
+      <c r="B581">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2">
+      <c r="A582" s="3">
+        <v>44640</v>
+      </c>
+      <c r="B582">
+        <v>7.48</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2">
+      <c r="A583" s="3">
+        <v>44641</v>
+      </c>
+      <c r="B583">
+        <v>7.44</v>
+      </c>
+    </row>
+    <row r="584" spans="1:2">
+      <c r="A584" s="3">
+        <v>44642</v>
+      </c>
+      <c r="B584">
+        <v>7.46</v>
+      </c>
+    </row>
+    <row r="585" spans="1:2">
+      <c r="A585" s="3">
+        <v>44643</v>
+      </c>
+      <c r="B585">
+        <v>7.29</v>
+      </c>
+    </row>
+    <row r="586" spans="1:2">
+      <c r="A586" s="3">
+        <v>44644</v>
+      </c>
+      <c r="B586">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="587" spans="1:2">
+      <c r="A587" s="3">
+        <v>44645</v>
+      </c>
+      <c r="B587">
+        <v>7.29</v>
+      </c>
+    </row>
+    <row r="588" spans="1:2">
+      <c r="A588" s="3">
+        <v>44646</v>
+      </c>
+      <c r="B588">
+        <v>7.39</v>
       </c>
     </row>
   </sheetData>
@@ -48896,7 +50049,7 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView zoomScale="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:D6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -48983,13 +50136,13 @@
         <v>126</v>
       </c>
       <c r="B6" s="31">
-        <v>6.9000000000000006E-2</v>
+        <v>0.158</v>
       </c>
       <c r="C6" s="31">
-        <v>-0.28699999999999998</v>
+        <v>-0.255</v>
       </c>
       <c r="D6" s="31">
-        <v>-3.2000000000000001E-2</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="F6" s="26"/>
     </row>
@@ -49357,11 +50510,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE529FD-4597-F641-B496-01BE3204D79B}">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E128" sqref="E128"/>
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -49384,7 +50537,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4">
+      <c r="A2" s="25">
         <v>43744</v>
       </c>
       <c r="B2">
@@ -49398,7 +50551,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="4">
+      <c r="A3" s="25">
         <v>43751</v>
       </c>
       <c r="B3">
@@ -49412,7 +50565,7 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="4">
+      <c r="A4" s="25">
         <v>43758</v>
       </c>
       <c r="B4">
@@ -49426,7 +50579,7 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="4">
+      <c r="A5" s="25">
         <v>43765</v>
       </c>
       <c r="B5">
@@ -49440,7 +50593,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="4">
+      <c r="A6" s="25">
         <v>43772</v>
       </c>
       <c r="B6">
@@ -49454,7 +50607,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="4">
+      <c r="A7" s="25">
         <v>43779</v>
       </c>
       <c r="B7">
@@ -49468,7 +50621,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="4">
+      <c r="A8" s="25">
         <v>43786</v>
       </c>
       <c r="B8">
@@ -49482,7 +50635,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="4">
+      <c r="A9" s="25">
         <v>43793</v>
       </c>
       <c r="B9">
@@ -49496,7 +50649,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="4">
+      <c r="A10" s="25">
         <v>43800</v>
       </c>
       <c r="B10">
@@ -49510,7 +50663,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="4">
+      <c r="A11" s="25">
         <v>43807</v>
       </c>
       <c r="B11">
@@ -49524,7 +50677,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="4">
+      <c r="A12" s="25">
         <v>43814</v>
       </c>
       <c r="B12">
@@ -49538,7 +50691,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="4">
+      <c r="A13" s="25">
         <v>43821</v>
       </c>
       <c r="B13">
@@ -49552,7 +50705,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="4">
+      <c r="A14" s="25">
         <v>43828</v>
       </c>
       <c r="B14">
@@ -49566,7 +50719,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="4">
+      <c r="A15" s="25">
         <v>43835</v>
       </c>
       <c r="B15">
@@ -49580,7 +50733,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="4">
+      <c r="A16" s="25">
         <v>43842</v>
       </c>
       <c r="B16">
@@ -49594,7 +50747,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="4">
+      <c r="A17" s="25">
         <v>43849</v>
       </c>
       <c r="B17">
@@ -49608,7 +50761,7 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="4">
+      <c r="A18" s="25">
         <v>43856</v>
       </c>
       <c r="B18">
@@ -49622,7 +50775,7 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="4">
+      <c r="A19" s="25">
         <v>43863</v>
       </c>
       <c r="B19">
@@ -49636,7 +50789,7 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="4">
+      <c r="A20" s="25">
         <v>43870</v>
       </c>
       <c r="B20">
@@ -49650,7 +50803,7 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="4">
+      <c r="A21" s="25">
         <v>43877</v>
       </c>
       <c r="B21">
@@ -49664,7 +50817,7 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="4">
+      <c r="A22" s="25">
         <v>43884</v>
       </c>
       <c r="B22">
@@ -49678,7 +50831,7 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="4">
+      <c r="A23" s="25">
         <v>43891</v>
       </c>
       <c r="B23">
@@ -49692,7 +50845,7 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="4">
+      <c r="A24" s="25">
         <v>43898</v>
       </c>
       <c r="B24">
@@ -49706,7 +50859,7 @@
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="4">
+      <c r="A25" s="25">
         <v>43905</v>
       </c>
       <c r="B25">
@@ -49720,7 +50873,7 @@
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="4">
+      <c r="A26" s="25">
         <v>43912</v>
       </c>
       <c r="B26">
@@ -49734,7 +50887,7 @@
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="4">
+      <c r="A27" s="25">
         <v>43919</v>
       </c>
       <c r="B27">
@@ -49748,7 +50901,7 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="4">
+      <c r="A28" s="25">
         <v>43926</v>
       </c>
       <c r="B28">
@@ -49762,7 +50915,7 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="4">
+      <c r="A29" s="25">
         <v>43933</v>
       </c>
       <c r="B29">
@@ -49776,7 +50929,7 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="4">
+      <c r="A30" s="25">
         <v>43940</v>
       </c>
       <c r="B30">
@@ -49790,7 +50943,7 @@
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="4">
+      <c r="A31" s="25">
         <v>43947</v>
       </c>
       <c r="B31">
@@ -49804,7 +50957,7 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="4">
+      <c r="A32" s="25">
         <v>43954</v>
       </c>
       <c r="B32">
@@ -49818,7 +50971,7 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="4">
+      <c r="A33" s="25">
         <v>43961</v>
       </c>
       <c r="B33">
@@ -49832,7 +50985,7 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="4">
+      <c r="A34" s="25">
         <v>43968</v>
       </c>
       <c r="B34">
@@ -49846,7 +50999,7 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="4">
+      <c r="A35" s="25">
         <v>43975</v>
       </c>
       <c r="B35">
@@ -49860,7 +51013,7 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="4">
+      <c r="A36" s="25">
         <v>43982</v>
       </c>
       <c r="B36">
@@ -49874,7 +51027,7 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="4">
+      <c r="A37" s="25">
         <v>43989</v>
       </c>
       <c r="B37">
@@ -49888,7 +51041,7 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="4">
+      <c r="A38" s="25">
         <v>43996</v>
       </c>
       <c r="B38">
@@ -49902,7 +51055,7 @@
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="4">
+      <c r="A39" s="25">
         <v>44003</v>
       </c>
       <c r="B39">
@@ -49916,7 +51069,7 @@
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="4">
+      <c r="A40" s="25">
         <v>44010</v>
       </c>
       <c r="B40">
@@ -49930,7 +51083,7 @@
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="4">
+      <c r="A41" s="25">
         <v>44017</v>
       </c>
       <c r="B41">
@@ -49944,7 +51097,7 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="4">
+      <c r="A42" s="25">
         <v>44024</v>
       </c>
       <c r="B42">
@@ -49958,7 +51111,7 @@
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="4">
+      <c r="A43" s="25">
         <v>44031</v>
       </c>
       <c r="B43">
@@ -49972,7 +51125,7 @@
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="4">
+      <c r="A44" s="25">
         <v>44038</v>
       </c>
       <c r="B44">
@@ -49986,7 +51139,7 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="4">
+      <c r="A45" s="25">
         <v>44045</v>
       </c>
       <c r="B45">
@@ -50000,7 +51153,7 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="4">
+      <c r="A46" s="25">
         <v>44052</v>
       </c>
       <c r="B46">
@@ -50014,7 +51167,7 @@
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="4">
+      <c r="A47" s="25">
         <v>44059</v>
       </c>
       <c r="B47">
@@ -50028,7 +51181,7 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="4">
+      <c r="A48" s="25">
         <v>44066</v>
       </c>
       <c r="B48">
@@ -50042,7 +51195,7 @@
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="4">
+      <c r="A49" s="25">
         <v>44073</v>
       </c>
       <c r="B49">
@@ -50056,7 +51209,7 @@
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="4">
+      <c r="A50" s="25">
         <v>44080</v>
       </c>
       <c r="B50">
@@ -50070,7 +51223,7 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="4">
+      <c r="A51" s="25">
         <v>44087</v>
       </c>
       <c r="B51">
@@ -50084,7 +51237,7 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="4">
+      <c r="A52" s="25">
         <v>44094</v>
       </c>
       <c r="B52">
@@ -50098,7 +51251,7 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="4">
+      <c r="A53" s="25">
         <v>44101</v>
       </c>
       <c r="B53">
@@ -50112,7 +51265,7 @@
       </c>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="4">
+      <c r="A54" s="25">
         <v>44108</v>
       </c>
       <c r="B54">
@@ -50126,7 +51279,7 @@
       </c>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="4">
+      <c r="A55" s="25">
         <v>44115</v>
       </c>
       <c r="B55">
@@ -50140,7 +51293,7 @@
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="4">
+      <c r="A56" s="25">
         <v>44122</v>
       </c>
       <c r="B56">
@@ -50154,7 +51307,7 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="4">
+      <c r="A57" s="25">
         <v>44129</v>
       </c>
       <c r="B57">
@@ -50168,7 +51321,7 @@
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="4">
+      <c r="A58" s="25">
         <v>44136</v>
       </c>
       <c r="B58">
@@ -50182,7 +51335,7 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="4">
+      <c r="A59" s="25">
         <v>44143</v>
       </c>
       <c r="B59">
@@ -50196,7 +51349,7 @@
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="4">
+      <c r="A60" s="25">
         <v>44150</v>
       </c>
       <c r="B60">
@@ -50210,7 +51363,7 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="4">
+      <c r="A61" s="25">
         <v>44157</v>
       </c>
       <c r="B61">
@@ -50224,7 +51377,7 @@
       </c>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="4">
+      <c r="A62" s="25">
         <v>44164</v>
       </c>
       <c r="B62">
@@ -50241,7 +51394,7 @@
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="4">
+      <c r="A63" s="25">
         <v>44171</v>
       </c>
       <c r="B63">
@@ -50258,7 +51411,7 @@
       </c>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="4">
+      <c r="A64" s="25">
         <v>44178</v>
       </c>
       <c r="B64">
@@ -50275,7 +51428,7 @@
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="4">
+      <c r="A65" s="25">
         <v>44185</v>
       </c>
       <c r="B65">
@@ -50292,7 +51445,7 @@
       </c>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="4">
+      <c r="A66" s="25">
         <v>44192</v>
       </c>
       <c r="B66">
@@ -50309,7 +51462,7 @@
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="4">
+      <c r="A67" s="25">
         <v>44199</v>
       </c>
       <c r="B67">
@@ -50326,7 +51479,7 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="4">
+      <c r="A68" s="25">
         <v>44206</v>
       </c>
       <c r="B68">
@@ -50343,7 +51496,7 @@
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="4">
+      <c r="A69" s="25">
         <v>44213</v>
       </c>
       <c r="B69">
@@ -50360,7 +51513,7 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="4">
+      <c r="A70" s="25">
         <v>44220</v>
       </c>
       <c r="B70">
@@ -50373,11 +51526,11 @@
         <v>4.97</v>
       </c>
       <c r="E70">
-        <v>43.23</v>
+        <v>41.3</v>
       </c>
     </row>
     <row r="71" spans="1:5">
-      <c r="A71" s="4">
+      <c r="A71" s="25">
         <v>44227</v>
       </c>
       <c r="B71">
@@ -50390,11 +51543,11 @@
         <v>4.8899999999999997</v>
       </c>
       <c r="E71">
-        <v>41.68</v>
+        <v>40.57</v>
       </c>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="4">
+      <c r="A72" s="25">
         <v>44234</v>
       </c>
       <c r="B72">
@@ -50407,11 +51560,11 @@
         <v>8.0299999999999994</v>
       </c>
       <c r="E72">
-        <v>42.69</v>
+        <v>40.880000000000003</v>
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="4">
+      <c r="A73" s="25">
         <v>44241</v>
       </c>
       <c r="B73">
@@ -50424,11 +51577,11 @@
         <v>7.02</v>
       </c>
       <c r="E73">
-        <v>42.27</v>
+        <v>40.46</v>
       </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="4">
+      <c r="A74" s="25">
         <v>44248</v>
       </c>
       <c r="B74">
@@ -50441,11 +51594,11 @@
         <v>6.61</v>
       </c>
       <c r="E74">
-        <v>41.89</v>
+        <v>40.479999999999997</v>
       </c>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="4">
+      <c r="A75" s="25">
         <v>44255</v>
       </c>
       <c r="B75">
@@ -50458,11 +51611,11 @@
         <v>6.82</v>
       </c>
       <c r="E75">
-        <v>42.44</v>
+        <v>40.61</v>
       </c>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="4">
+      <c r="A76" s="25">
         <v>44262</v>
       </c>
       <c r="B76">
@@ -50475,11 +51628,11 @@
         <v>5.86</v>
       </c>
       <c r="E76">
-        <v>41.52</v>
+        <v>39.770000000000003</v>
       </c>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="4">
+      <c r="A77" s="25">
         <v>44269</v>
       </c>
       <c r="B77">
@@ -50492,11 +51645,11 @@
         <v>6.17</v>
       </c>
       <c r="E77">
-        <v>40.81</v>
+        <v>39.49</v>
       </c>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="4">
+      <c r="A78" s="25">
         <v>44276</v>
       </c>
       <c r="B78">
@@ -50509,11 +51662,11 @@
         <v>6.51</v>
       </c>
       <c r="E78">
-        <v>42.23</v>
+        <v>40.590000000000003</v>
       </c>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="4">
+      <c r="A79" s="25">
         <v>44283</v>
       </c>
       <c r="B79">
@@ -50526,11 +51679,11 @@
         <v>6.18</v>
       </c>
       <c r="E79">
-        <v>43.46</v>
+        <v>41.21</v>
       </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="4">
+      <c r="A80" s="25">
         <v>44290</v>
       </c>
       <c r="B80">
@@ -50543,11 +51696,11 @@
         <v>8.58</v>
       </c>
       <c r="E80">
-        <v>43</v>
+        <v>41.19</v>
       </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="4">
+      <c r="A81" s="25">
         <v>44297</v>
       </c>
       <c r="B81">
@@ -50560,11 +51713,11 @@
         <v>8</v>
       </c>
       <c r="E81">
-        <v>41.23</v>
+        <v>40.06</v>
       </c>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="4">
+      <c r="A82" s="25">
         <v>44304</v>
       </c>
       <c r="B82">
@@ -50577,11 +51730,11 @@
         <v>7.31</v>
       </c>
       <c r="E82">
-        <v>41.35</v>
+        <v>40.18</v>
       </c>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="4">
+      <c r="A83" s="25">
         <v>44311</v>
       </c>
       <c r="B83">
@@ -50594,11 +51747,11 @@
         <v>6.37</v>
       </c>
       <c r="E83">
-        <v>40.83</v>
+        <v>40.049999999999997</v>
       </c>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="4">
+      <c r="A84" s="25">
         <v>44318</v>
       </c>
       <c r="B84">
@@ -50611,11 +51764,11 @@
         <v>7.35</v>
       </c>
       <c r="E84">
-        <v>40.630000000000003</v>
+        <v>38.93</v>
       </c>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="4">
+      <c r="A85" s="25">
         <v>44325</v>
       </c>
       <c r="B85">
@@ -50628,11 +51781,11 @@
         <v>7.29</v>
       </c>
       <c r="E85">
-        <v>42.97</v>
+        <v>41.3</v>
       </c>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="4">
+      <c r="A86" s="25">
         <v>44332</v>
       </c>
       <c r="B86">
@@ -50645,11 +51798,11 @@
         <v>14.34</v>
       </c>
       <c r="E86">
-        <v>42.33</v>
+        <v>40.53</v>
       </c>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="4">
+      <c r="A87" s="25">
         <v>44339</v>
       </c>
       <c r="B87">
@@ -50662,11 +51815,11 @@
         <v>13.52</v>
       </c>
       <c r="E87">
-        <v>41</v>
+        <v>39.380000000000003</v>
       </c>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="4">
+      <c r="A88" s="25">
         <v>44346</v>
       </c>
       <c r="B88">
@@ -50679,11 +51832,11 @@
         <v>9.58</v>
       </c>
       <c r="E88">
-        <v>40.61</v>
+        <v>38.950000000000003</v>
       </c>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="4">
+      <c r="A89" s="25">
         <v>44353</v>
       </c>
       <c r="B89">
@@ -50696,11 +51849,11 @@
         <v>13.27</v>
       </c>
       <c r="E89">
-        <v>40.9</v>
+        <v>39.24</v>
       </c>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="4">
+      <c r="A90" s="25">
         <v>44360</v>
       </c>
       <c r="B90">
@@ -50713,11 +51866,11 @@
         <v>8.23</v>
       </c>
       <c r="E90">
-        <v>40.89</v>
+        <v>39.75</v>
       </c>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="4">
+      <c r="A91" s="25">
         <v>44367</v>
       </c>
       <c r="B91">
@@ -50730,11 +51883,11 @@
         <v>8.92</v>
       </c>
       <c r="E91">
-        <v>42.13</v>
+        <v>40.49</v>
       </c>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="4">
+      <c r="A92" s="25">
         <v>44374</v>
       </c>
       <c r="B92">
@@ -50747,11 +51900,11 @@
         <v>8.6</v>
       </c>
       <c r="E92">
-        <v>40.92</v>
+        <v>39.6</v>
       </c>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="4">
+      <c r="A93" s="25">
         <v>44381</v>
       </c>
       <c r="B93">
@@ -50764,11 +51917,11 @@
         <v>6.71</v>
       </c>
       <c r="E93">
-        <v>40.85</v>
+        <v>39.49</v>
       </c>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="4">
+      <c r="A94" s="25">
         <v>44388</v>
       </c>
       <c r="B94">
@@ -50781,11 +51934,11 @@
         <v>7.06</v>
       </c>
       <c r="E94">
-        <v>41.94</v>
+        <v>40.590000000000003</v>
       </c>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="4">
+      <c r="A95" s="25">
         <v>44395</v>
       </c>
       <c r="B95">
@@ -50798,11 +51951,11 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E95">
-        <v>42.06</v>
+        <v>40.409999999999997</v>
       </c>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="4">
+      <c r="A96" s="25">
         <v>44402</v>
       </c>
       <c r="B96">
@@ -50815,11 +51968,11 @@
         <v>6.75</v>
       </c>
       <c r="E96">
-        <v>42.82</v>
+        <v>41.13</v>
       </c>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="4">
+      <c r="A97" s="25">
         <v>44409</v>
       </c>
       <c r="B97">
@@ -50832,11 +51985,11 @@
         <v>7.18</v>
       </c>
       <c r="E97">
-        <v>41.25</v>
+        <v>39.78</v>
       </c>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="4">
+      <c r="A98" s="25">
         <v>44416</v>
       </c>
       <c r="B98">
@@ -50849,11 +52002,11 @@
         <v>7.27</v>
       </c>
       <c r="E98">
-        <v>43.29</v>
+        <v>41.48</v>
       </c>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="4">
+      <c r="A99" s="25">
         <v>44423</v>
       </c>
       <c r="B99">
@@ -50866,11 +52019,11 @@
         <v>7.01</v>
       </c>
       <c r="E99">
-        <v>41.77</v>
+        <v>40.42</v>
       </c>
     </row>
     <row r="100" spans="1:5">
-      <c r="A100" s="4">
+      <c r="A100" s="25">
         <v>44430</v>
       </c>
       <c r="B100">
@@ -50883,11 +52036,11 @@
         <v>7.34</v>
       </c>
       <c r="E100">
-        <v>40.93</v>
+        <v>40.020000000000003</v>
       </c>
     </row>
     <row r="101" spans="1:5">
-      <c r="A101" s="4">
+      <c r="A101" s="25">
         <v>44437</v>
       </c>
       <c r="B101">
@@ -50900,11 +52053,11 @@
         <v>8.4600000000000009</v>
       </c>
       <c r="E101">
-        <v>42.23</v>
+        <v>40.78</v>
       </c>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="4">
+      <c r="A102" s="25">
         <v>44444</v>
       </c>
       <c r="B102">
@@ -50917,11 +52070,11 @@
         <v>8.6199999999999992</v>
       </c>
       <c r="E102">
-        <v>42.48</v>
+        <v>41.04</v>
       </c>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="4">
+      <c r="A103" s="25">
         <v>44451</v>
       </c>
       <c r="B103">
@@ -50934,11 +52087,11 @@
         <v>6.51</v>
       </c>
       <c r="E103">
-        <v>42.45</v>
+        <v>40.869999999999997</v>
       </c>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="4">
+      <c r="A104" s="25">
         <v>44458</v>
       </c>
       <c r="B104">
@@ -50951,11 +52104,11 @@
         <v>4.92</v>
       </c>
       <c r="E104">
-        <v>40.770000000000003</v>
+        <v>39.75</v>
       </c>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="4">
+      <c r="A105" s="25">
         <v>44465</v>
       </c>
       <c r="B105">
@@ -50968,11 +52121,11 @@
         <v>5.36</v>
       </c>
       <c r="E105">
-        <v>43.23</v>
+        <v>41.3</v>
       </c>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="4">
+      <c r="A106" s="25">
         <v>44472</v>
       </c>
       <c r="B106">
@@ -50985,11 +52138,11 @@
         <v>6.99</v>
       </c>
       <c r="E106">
-        <v>39.799999999999997</v>
+        <v>39.229999999999997</v>
       </c>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="4">
+      <c r="A107" s="25">
         <v>44479</v>
       </c>
       <c r="B107">
@@ -51002,11 +52155,11 @@
         <v>9.48</v>
       </c>
       <c r="E107">
-        <v>42.07</v>
+        <v>40.409999999999997</v>
       </c>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="4">
+      <c r="A108" s="25">
         <v>44486</v>
       </c>
       <c r="B108">
@@ -51019,11 +52172,11 @@
         <v>7.23</v>
       </c>
       <c r="E108">
-        <v>43.47</v>
+        <v>41.56</v>
       </c>
     </row>
     <row r="109" spans="1:5">
-      <c r="A109" s="4">
+      <c r="A109" s="25">
         <v>44493</v>
       </c>
       <c r="B109">
@@ -51036,11 +52189,11 @@
         <v>7.8</v>
       </c>
       <c r="E109">
-        <v>42.22</v>
+        <v>40.659999999999997</v>
       </c>
     </row>
     <row r="110" spans="1:5">
-      <c r="A110" s="4">
+      <c r="A110" s="25">
         <v>44500</v>
       </c>
       <c r="B110">
@@ -51053,11 +52206,11 @@
         <v>7.02</v>
       </c>
       <c r="E110">
-        <v>41.41</v>
+        <v>39.93</v>
       </c>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="4">
+      <c r="A111" s="25">
         <v>44507</v>
       </c>
       <c r="B111">
@@ -51070,11 +52223,11 @@
         <v>6.34</v>
       </c>
       <c r="E111">
-        <v>41.23</v>
+        <v>39.729999999999997</v>
       </c>
     </row>
     <row r="112" spans="1:5">
-      <c r="A112" s="4">
+      <c r="A112" s="25">
         <v>44514</v>
       </c>
       <c r="B112">
@@ -51087,11 +52240,11 @@
         <v>6.31</v>
       </c>
       <c r="E112">
-        <v>41.1</v>
+        <v>39.67</v>
       </c>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="4">
+      <c r="A113" s="25">
         <v>44521</v>
       </c>
       <c r="B113">
@@ -51104,11 +52257,11 @@
         <v>7.04</v>
       </c>
       <c r="E113">
-        <v>41.04</v>
+        <v>39.79</v>
       </c>
     </row>
     <row r="114" spans="1:5">
-      <c r="A114" s="4">
+      <c r="A114" s="25">
         <v>44528</v>
       </c>
       <c r="B114">
@@ -51121,11 +52274,11 @@
         <v>6.11</v>
       </c>
       <c r="E114">
-        <v>41.72</v>
+        <v>40.51</v>
       </c>
     </row>
     <row r="115" spans="1:5">
-      <c r="A115" s="4">
+      <c r="A115" s="25">
         <v>44505</v>
       </c>
       <c r="B115">
@@ -51138,11 +52291,11 @@
         <v>6.53</v>
       </c>
       <c r="E115">
-        <v>41.95</v>
+        <v>40.450000000000003</v>
       </c>
     </row>
     <row r="116" spans="1:5">
-      <c r="A116" s="4">
+      <c r="A116" s="25">
         <v>44542</v>
       </c>
       <c r="B116">
@@ -51155,11 +52308,11 @@
         <v>7.82</v>
       </c>
       <c r="E116">
-        <v>42.96</v>
+        <v>41.39</v>
       </c>
     </row>
     <row r="117" spans="1:5">
-      <c r="A117" s="4">
+      <c r="A117" s="25">
         <v>44549</v>
       </c>
       <c r="B117">
@@ -51172,11 +52325,11 @@
         <v>7.12</v>
       </c>
       <c r="E117">
-        <v>42.23</v>
+        <v>40.86</v>
       </c>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="4">
+      <c r="A118" s="25">
         <v>44556</v>
       </c>
       <c r="B118">
@@ -51189,11 +52342,11 @@
         <v>7.08</v>
       </c>
       <c r="E118">
-        <v>42.24</v>
+        <v>40.729999999999997</v>
       </c>
     </row>
     <row r="119" spans="1:5">
-      <c r="A119" s="4">
+      <c r="A119" s="25">
         <v>44563</v>
       </c>
       <c r="B119">
@@ -51206,11 +52359,11 @@
         <v>5.35</v>
       </c>
       <c r="E119">
-        <v>41.86</v>
+        <v>40.58</v>
       </c>
     </row>
     <row r="120" spans="1:5">
-      <c r="A120" s="4">
+      <c r="A120" s="25">
         <v>44570</v>
       </c>
       <c r="B120">
@@ -51223,11 +52376,11 @@
         <v>6.68</v>
       </c>
       <c r="E120">
-        <v>41.39</v>
+        <v>40.049999999999997</v>
       </c>
     </row>
     <row r="121" spans="1:5">
-      <c r="A121" s="4">
+      <c r="A121" s="25">
         <v>44577</v>
       </c>
       <c r="B121">
@@ -51240,11 +52393,11 @@
         <v>4.99</v>
       </c>
       <c r="E121">
-        <v>40.700000000000003</v>
+        <v>39.65</v>
       </c>
     </row>
     <row r="122" spans="1:5">
-      <c r="A122" s="4">
+      <c r="A122" s="25">
         <v>44584</v>
       </c>
       <c r="B122">
@@ -51255,7 +52408,7 @@
       </c>
     </row>
     <row r="123" spans="1:5">
-      <c r="A123" s="4">
+      <c r="A123" s="25">
         <v>44591</v>
       </c>
       <c r="B123">
@@ -51266,7 +52419,7 @@
       </c>
     </row>
     <row r="124" spans="1:5">
-      <c r="A124" s="4">
+      <c r="A124" s="25">
         <v>44598</v>
       </c>
       <c r="B124">
@@ -51277,7 +52430,7 @@
       </c>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="4">
+      <c r="A125" s="25">
         <v>44605</v>
       </c>
       <c r="B125">
@@ -51288,7 +52441,7 @@
       </c>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" s="3">
+      <c r="A126" s="25">
         <v>44612</v>
       </c>
       <c r="B126">
@@ -51299,7 +52452,7 @@
       </c>
     </row>
     <row r="127" spans="1:5">
-      <c r="A127" s="3">
+      <c r="A127" s="25">
         <v>44619</v>
       </c>
       <c r="B127">
@@ -51310,7 +52463,7 @@
       </c>
     </row>
     <row r="128" spans="1:5">
-      <c r="A128" s="3">
+      <c r="A128" s="25">
         <v>44626</v>
       </c>
       <c r="B128">
@@ -51318,6 +52471,28 @@
       </c>
       <c r="E128">
         <v>39.49</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="25">
+        <v>44633</v>
+      </c>
+      <c r="B129">
+        <v>7.73</v>
+      </c>
+      <c r="E129">
+        <v>39.01</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" s="25">
+        <v>44640</v>
+      </c>
+      <c r="B130">
+        <v>7.86</v>
+      </c>
+      <c r="E130">
+        <v>39.29</v>
       </c>
     </row>
   </sheetData>
@@ -51327,10 +52502,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D5DA751-8DDE-2444-A8CE-DEF963043B5D}">
-  <dimension ref="A1:J404"/>
+  <dimension ref="A1:J418"/>
   <sheetViews>
-    <sheetView topLeftCell="A396" workbookViewId="0">
-      <selection activeCell="B397" sqref="B397"/>
+    <sheetView topLeftCell="A399" workbookViewId="0">
+      <selection activeCell="B413" sqref="B413"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -64261,6 +65436,454 @@
       </c>
       <c r="J404">
         <v>67.16</v>
+      </c>
+    </row>
+    <row r="405" spans="1:10">
+      <c r="A405" s="3">
+        <v>44633</v>
+      </c>
+      <c r="B405">
+        <v>64.36</v>
+      </c>
+      <c r="C405">
+        <v>57.17</v>
+      </c>
+      <c r="D405">
+        <v>67.7</v>
+      </c>
+      <c r="E405">
+        <v>64.25</v>
+      </c>
+      <c r="F405">
+        <v>55.65</v>
+      </c>
+      <c r="G405">
+        <v>68.540000000000006</v>
+      </c>
+      <c r="H405">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="I405">
+        <v>58.17</v>
+      </c>
+      <c r="J405">
+        <v>67.16</v>
+      </c>
+    </row>
+    <row r="406" spans="1:10">
+      <c r="A406" s="3">
+        <v>44634</v>
+      </c>
+      <c r="B406">
+        <v>64.36</v>
+      </c>
+      <c r="C406">
+        <v>57.33</v>
+      </c>
+      <c r="D406">
+        <v>67.7</v>
+      </c>
+      <c r="E406">
+        <v>64.25</v>
+      </c>
+      <c r="F406">
+        <v>55.65</v>
+      </c>
+      <c r="G406">
+        <v>68.540000000000006</v>
+      </c>
+      <c r="H406">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="I406">
+        <v>58.45</v>
+      </c>
+      <c r="J406">
+        <v>67.16</v>
+      </c>
+    </row>
+    <row r="407" spans="1:10">
+      <c r="A407" s="3">
+        <v>44635</v>
+      </c>
+      <c r="B407">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="C407">
+        <v>58</v>
+      </c>
+      <c r="D407">
+        <v>67.52</v>
+      </c>
+      <c r="E407">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="F407">
+        <v>56.49</v>
+      </c>
+      <c r="G407">
+        <v>68.540000000000006</v>
+      </c>
+      <c r="H407">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="I407">
+        <v>59</v>
+      </c>
+      <c r="J407">
+        <v>66.87</v>
+      </c>
+    </row>
+    <row r="408" spans="1:10">
+      <c r="A408" s="3">
+        <v>44636</v>
+      </c>
+      <c r="B408">
+        <v>64.72</v>
+      </c>
+      <c r="C408">
+        <v>58.17</v>
+      </c>
+      <c r="D408">
+        <v>67.52</v>
+      </c>
+      <c r="E408">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="F408">
+        <v>56.49</v>
+      </c>
+      <c r="G408">
+        <v>68.540000000000006</v>
+      </c>
+      <c r="H408">
+        <v>64.72</v>
+      </c>
+      <c r="I408">
+        <v>59.28</v>
+      </c>
+      <c r="J408">
+        <v>66.87</v>
+      </c>
+    </row>
+    <row r="409" spans="1:10">
+      <c r="A409" s="3">
+        <v>44637</v>
+      </c>
+      <c r="B409">
+        <v>64.72</v>
+      </c>
+      <c r="C409">
+        <v>58.17</v>
+      </c>
+      <c r="D409">
+        <v>67.52</v>
+      </c>
+      <c r="E409">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="F409">
+        <v>56.49</v>
+      </c>
+      <c r="G409">
+        <v>68.540000000000006</v>
+      </c>
+      <c r="H409">
+        <v>64.72</v>
+      </c>
+      <c r="I409">
+        <v>59.28</v>
+      </c>
+      <c r="J409">
+        <v>66.87</v>
+      </c>
+    </row>
+    <row r="410" spans="1:10">
+      <c r="A410" s="3">
+        <v>44638</v>
+      </c>
+      <c r="B410">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="C410">
+        <v>58.17</v>
+      </c>
+      <c r="D410">
+        <v>67.88</v>
+      </c>
+      <c r="E410">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="F410">
+        <v>56.9</v>
+      </c>
+      <c r="G410">
+        <v>69.010000000000005</v>
+      </c>
+      <c r="H410">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="I410">
+        <v>59</v>
+      </c>
+      <c r="J410">
+        <v>67.16</v>
+      </c>
+    </row>
+    <row r="411" spans="1:10">
+      <c r="A411" s="3">
+        <v>44639</v>
+      </c>
+      <c r="B411">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="C411">
+        <v>58</v>
+      </c>
+      <c r="D411">
+        <v>67.88</v>
+      </c>
+      <c r="E411">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="F411">
+        <v>56.49</v>
+      </c>
+      <c r="G411">
+        <v>69.010000000000005</v>
+      </c>
+      <c r="H411">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="I411">
+        <v>59</v>
+      </c>
+      <c r="J411">
+        <v>67.16</v>
+      </c>
+    </row>
+    <row r="412" spans="1:10">
+      <c r="A412" s="3">
+        <v>44640</v>
+      </c>
+      <c r="B412">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="C412">
+        <v>58</v>
+      </c>
+      <c r="D412">
+        <v>68.069999999999993</v>
+      </c>
+      <c r="E412">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="F412">
+        <v>56.49</v>
+      </c>
+      <c r="G412">
+        <v>69.010000000000005</v>
+      </c>
+      <c r="H412">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="I412">
+        <v>59</v>
+      </c>
+      <c r="J412">
+        <v>67.459999999999994</v>
+      </c>
+    </row>
+    <row r="413" spans="1:10">
+      <c r="A413" s="3">
+        <v>44641</v>
+      </c>
+      <c r="B413">
+        <v>64.540000000000006</v>
+      </c>
+      <c r="C413">
+        <v>58.17</v>
+      </c>
+      <c r="D413">
+        <v>67.7</v>
+      </c>
+      <c r="E413">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="F413">
+        <v>56.9</v>
+      </c>
+      <c r="G413">
+        <v>69.010000000000005</v>
+      </c>
+      <c r="H413">
+        <v>64.430000000000007</v>
+      </c>
+      <c r="I413">
+        <v>59</v>
+      </c>
+      <c r="J413">
+        <v>66.87</v>
+      </c>
+    </row>
+    <row r="414" spans="1:10">
+      <c r="A414" s="3">
+        <v>44642</v>
+      </c>
+      <c r="B414">
+        <v>64.72</v>
+      </c>
+      <c r="C414">
+        <v>57.83</v>
+      </c>
+      <c r="D414">
+        <v>68.069999999999993</v>
+      </c>
+      <c r="E414">
+        <v>64.709999999999994</v>
+      </c>
+      <c r="F414">
+        <v>56.49</v>
+      </c>
+      <c r="G414">
+        <v>69.010000000000005</v>
+      </c>
+      <c r="H414">
+        <v>64.72</v>
+      </c>
+      <c r="I414">
+        <v>58.73</v>
+      </c>
+      <c r="J414">
+        <v>67.459999999999994</v>
+      </c>
+    </row>
+    <row r="415" spans="1:10">
+      <c r="A415" s="3">
+        <v>44643</v>
+      </c>
+      <c r="B415">
+        <v>65.069999999999993</v>
+      </c>
+      <c r="C415">
+        <v>58.17</v>
+      </c>
+      <c r="D415">
+        <v>68.430000000000007</v>
+      </c>
+      <c r="E415">
+        <v>65.16</v>
+      </c>
+      <c r="F415">
+        <v>56.9</v>
+      </c>
+      <c r="G415">
+        <v>69.48</v>
+      </c>
+      <c r="H415">
+        <v>65.010000000000005</v>
+      </c>
+      <c r="I415">
+        <v>59</v>
+      </c>
+      <c r="J415">
+        <v>67.760000000000005</v>
+      </c>
+    </row>
+    <row r="416" spans="1:10">
+      <c r="A416" s="3">
+        <v>44644</v>
+      </c>
+      <c r="B416">
+        <v>64.89</v>
+      </c>
+      <c r="C416">
+        <v>58</v>
+      </c>
+      <c r="D416">
+        <v>68.430000000000007</v>
+      </c>
+      <c r="E416">
+        <v>65.16</v>
+      </c>
+      <c r="F416">
+        <v>56.9</v>
+      </c>
+      <c r="G416">
+        <v>69.48</v>
+      </c>
+      <c r="H416">
+        <v>64.72</v>
+      </c>
+      <c r="I416">
+        <v>58.73</v>
+      </c>
+      <c r="J416">
+        <v>67.760000000000005</v>
+      </c>
+    </row>
+    <row r="417" spans="1:10">
+      <c r="A417" s="3">
+        <v>44645</v>
+      </c>
+      <c r="B417">
+        <v>64.89</v>
+      </c>
+      <c r="C417">
+        <v>58</v>
+      </c>
+      <c r="D417">
+        <v>68.25</v>
+      </c>
+      <c r="E417">
+        <v>65.16</v>
+      </c>
+      <c r="F417">
+        <v>57.32</v>
+      </c>
+      <c r="G417">
+        <v>69.010000000000005</v>
+      </c>
+      <c r="H417">
+        <v>64.72</v>
+      </c>
+      <c r="I417">
+        <v>58.45</v>
+      </c>
+      <c r="J417">
+        <v>67.760000000000005</v>
+      </c>
+    </row>
+    <row r="418" spans="1:10">
+      <c r="A418" s="3">
+        <v>44646</v>
+      </c>
+      <c r="B418">
+        <v>65.069999999999993</v>
+      </c>
+      <c r="C418">
+        <v>58</v>
+      </c>
+      <c r="D418">
+        <v>68.430000000000007</v>
+      </c>
+      <c r="E418">
+        <v>65.16</v>
+      </c>
+      <c r="F418">
+        <v>57.32</v>
+      </c>
+      <c r="G418">
+        <v>69.010000000000005</v>
+      </c>
+      <c r="H418">
+        <v>65.010000000000005</v>
+      </c>
+      <c r="I418">
+        <v>58.45</v>
+      </c>
+      <c r="J418">
+        <v>68.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>